<commit_message>
Se realizo la tarea de los circuitos
</commit_message>
<xml_diff>
--- a/Excel/clase 16 may2021.xlsx
+++ b/Excel/clase 16 may2021.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Luis\Documents\GitProjects\Clases-octave\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\terra\Documents\proyectosdegit\Clases-octave\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A43C8582-6044-4526-A0F3-6F1841F1D7D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E4584A-18B7-47F5-81A4-497F97C05BCA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{80487D3F-3748-420F-9EFB-E03356FF148D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{80487D3F-3748-420F-9EFB-E03356FF148D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Mininos cuadrados" sheetId="1" r:id="rId1"/>
+    <sheet name="Minimos Cuadrados" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -213,7 +213,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja2!$B$12</c:f>
+              <c:f>'Minimos Cuadrados'!$B$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -347,7 +347,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja2!$A$13:$A$18</c:f>
+              <c:f>'Minimos Cuadrados'!$A$13:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -374,7 +374,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja2!$B$13:$B$18</c:f>
+              <c:f>'Minimos Cuadrados'!$B$13:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1252,8 +1252,8 @@
       <xdr:row>15</xdr:row>
       <xdr:rowOff>133380</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="8" name="Entrada de lápiz 7">
@@ -1272,7 +1272,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="8" name="Entrada de lápiz 7">
@@ -1317,8 +1317,8 @@
       <xdr:row>16</xdr:row>
       <xdr:rowOff>19200</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="11" name="Entrada de lápiz 10">
@@ -1337,7 +1337,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="11" name="Entrada de lápiz 10">
@@ -1382,8 +1382,8 @@
       <xdr:row>15</xdr:row>
       <xdr:rowOff>133380</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="12" name="Entrada de lápiz 11">
@@ -1402,7 +1402,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="12" name="Entrada de lápiz 11">
@@ -1447,8 +1447,8 @@
       <xdr:row>17</xdr:row>
       <xdr:rowOff>148380</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="15" name="Entrada de lápiz 14">
@@ -1467,7 +1467,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="15" name="Entrada de lápiz 14">
@@ -1512,8 +1512,8 @@
       <xdr:row>23</xdr:row>
       <xdr:rowOff>1140</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="18" name="Entrada de lápiz 17">
@@ -1532,7 +1532,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="18" name="Entrada de lápiz 17">
@@ -1577,8 +1577,8 @@
       <xdr:row>23</xdr:row>
       <xdr:rowOff>146940</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="24" name="Entrada de lápiz 23">
@@ -1597,7 +1597,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="24" name="Entrada de lápiz 23">
@@ -1642,8 +1642,8 @@
       <xdr:row>23</xdr:row>
       <xdr:rowOff>59460</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="33" name="Entrada de lápiz 32">
@@ -1662,7 +1662,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="33" name="Entrada de lápiz 32">
@@ -1707,8 +1707,8 @@
       <xdr:row>23</xdr:row>
       <xdr:rowOff>50100</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="43" name="Entrada de lápiz 42">
@@ -1727,7 +1727,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="43" name="Entrada de lápiz 42">
@@ -1772,8 +1772,8 @@
       <xdr:row>22</xdr:row>
       <xdr:rowOff>68520</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="47" name="Entrada de lápiz 46">
@@ -1792,7 +1792,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="47" name="Entrada de lápiz 46">
@@ -1837,8 +1837,8 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>11520</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId21">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="60" name="Entrada de lápiz 59">
@@ -1857,7 +1857,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="60" name="Entrada de lápiz 59">
@@ -1902,8 +1902,8 @@
       <xdr:row>29</xdr:row>
       <xdr:rowOff>66300</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId23">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="67" name="Entrada de lápiz 66">
@@ -1922,7 +1922,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="67" name="Entrada de lápiz 66">
@@ -1967,8 +1967,8 @@
       <xdr:row>29</xdr:row>
       <xdr:rowOff>151620</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId25">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="75" name="Entrada de lápiz 74">
@@ -1987,7 +1987,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="75" name="Entrada de lápiz 74">
@@ -2032,8 +2032,8 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>151320</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId27">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="76" name="Entrada de lápiz 75">
@@ -2052,7 +2052,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="76" name="Entrada de lápiz 75">
@@ -2097,8 +2097,8 @@
       <xdr:row>30</xdr:row>
       <xdr:rowOff>15120</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId29">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="88" name="Entrada de lápiz 87">
@@ -2117,7 +2117,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="88" name="Entrada de lápiz 87">
@@ -2162,8 +2162,8 @@
       <xdr:row>29</xdr:row>
       <xdr:rowOff>123540</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId31">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="97" name="Entrada de lápiz 96">
@@ -2182,7 +2182,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="97" name="Entrada de lápiz 96">
@@ -2227,8 +2227,8 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>124320</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId33">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="98" name="Entrada de lápiz 97">
@@ -2247,7 +2247,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="98" name="Entrada de lápiz 97">
@@ -2292,8 +2292,8 @@
       <xdr:row>17</xdr:row>
       <xdr:rowOff>141900</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId35">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="103" name="Entrada de lápiz 102">
@@ -2312,7 +2312,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="103" name="Entrada de lápiz 102">
@@ -2357,8 +2357,8 @@
       <xdr:row>13</xdr:row>
       <xdr:rowOff>4260</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId37">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="104" name="Entrada de lápiz 103">
@@ -2377,7 +2377,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="104" name="Entrada de lápiz 103">
@@ -2422,8 +2422,8 @@
       <xdr:row>17</xdr:row>
       <xdr:rowOff>163860</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId39">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="105" name="Entrada de lápiz 104">
@@ -2442,7 +2442,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="105" name="Entrada de lápiz 104">
@@ -2487,8 +2487,8 @@
       <xdr:row>16</xdr:row>
       <xdr:rowOff>76080</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId41">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="106" name="Entrada de lápiz 105">
@@ -2507,7 +2507,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="106" name="Entrada de lápiz 105">
@@ -2552,8 +2552,8 @@
       <xdr:row>27</xdr:row>
       <xdr:rowOff>33120</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId43">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="111" name="Entrada de lápiz 110">
@@ -2572,7 +2572,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="111" name="Entrada de lápiz 110">
@@ -2617,8 +2617,8 @@
       <xdr:row>31</xdr:row>
       <xdr:rowOff>39360</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId45">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="112" name="Entrada de lápiz 111">
@@ -2637,7 +2637,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="112" name="Entrada de lápiz 111">
@@ -2682,8 +2682,8 @@
       <xdr:row>29</xdr:row>
       <xdr:rowOff>176280</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId47">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="113" name="Entrada de lápiz 112">
@@ -2702,7 +2702,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="113" name="Entrada de lápiz 112">
@@ -2747,8 +2747,8 @@
       <xdr:row>35</xdr:row>
       <xdr:rowOff>135840</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId49">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="118" name="Entrada de lápiz 117">
@@ -2767,7 +2767,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="118" name="Entrada de lápiz 117">
@@ -2812,8 +2812,8 @@
       <xdr:row>34</xdr:row>
       <xdr:rowOff>112140</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId51">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="121" name="Entrada de lápiz 120">
@@ -2832,7 +2832,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="121" name="Entrada de lápiz 120">
@@ -2877,8 +2877,8 @@
       <xdr:row>35</xdr:row>
       <xdr:rowOff>142095</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId53">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="122" name="Entrada de lápiz 121">
@@ -2897,7 +2897,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="122" name="Entrada de lápiz 121">
@@ -2942,8 +2942,8 @@
       <xdr:row>36</xdr:row>
       <xdr:rowOff>5595</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId54">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="123" name="Entrada de lápiz 122">
@@ -2962,7 +2962,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="123" name="Entrada de lápiz 122">
@@ -3007,8 +3007,8 @@
       <xdr:row>35</xdr:row>
       <xdr:rowOff>114015</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId55">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="124" name="Entrada de lápiz 123">
@@ -3027,7 +3027,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="124" name="Entrada de lápiz 123">
@@ -3072,8 +3072,8 @@
       <xdr:row>34</xdr:row>
       <xdr:rowOff>114795</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId56">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="125" name="Entrada de lápiz 124">
@@ -3092,7 +3092,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="125" name="Entrada de lápiz 124">
@@ -3186,8 +3186,8 @@
       <xdr:row>8</xdr:row>
       <xdr:rowOff>180960</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="27" name="Entrada de lápiz 26">
@@ -3206,7 +3206,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="27" name="Entrada de lápiz 26">
@@ -3251,8 +3251,8 @@
       <xdr:row>8</xdr:row>
       <xdr:rowOff>66480</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="43" name="Entrada de lápiz 42">
@@ -3271,7 +3271,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="43" name="Entrada de lápiz 42">
@@ -3316,8 +3316,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>133500</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="46" name="Entrada de lápiz 45">
@@ -3336,7 +3336,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="46" name="Entrada de lápiz 45">
@@ -3381,8 +3381,8 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>129420</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="47" name="Entrada de lápiz 46">
@@ -3401,7 +3401,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="47" name="Entrada de lápiz 46">
@@ -3446,8 +3446,8 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>37260</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="48" name="Entrada de lápiz 47">
@@ -3466,7 +3466,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="48" name="Entrada de lápiz 47">
@@ -3511,8 +3511,8 @@
       <xdr:row>8</xdr:row>
       <xdr:rowOff>53880</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="55" name="Entrada de lápiz 54">
@@ -3531,7 +3531,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="55" name="Entrada de lápiz 54">
@@ -3576,8 +3576,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>183180</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="56" name="Entrada de lápiz 55">
@@ -3596,7 +3596,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="56" name="Entrada de lápiz 55">
@@ -3641,8 +3641,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>133860</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="57" name="Entrada de lápiz 56">
@@ -3661,7 +3661,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="57" name="Entrada de lápiz 56">
@@ -3706,8 +3706,8 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>73920</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="58" name="Entrada de lápiz 57">
@@ -3726,7 +3726,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="58" name="Entrada de lápiz 57">
@@ -3771,8 +3771,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>59340</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId20">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="59" name="Entrada de lápiz 58">
@@ -3791,7 +3791,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="59" name="Entrada de lápiz 58">
@@ -3836,8 +3836,8 @@
       <xdr:row>8</xdr:row>
       <xdr:rowOff>32640</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId22">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="60" name="Entrada de lápiz 59">
@@ -3856,7 +3856,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="60" name="Entrada de lápiz 59">
@@ -3901,8 +3901,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>166620</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId24">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="61" name="Entrada de lápiz 60">
@@ -3921,7 +3921,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="61" name="Entrada de lápiz 60">
@@ -3966,8 +3966,8 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>173340</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId26">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="64" name="Entrada de lápiz 63">
@@ -3986,7 +3986,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="64" name="Entrada de lápiz 63">
@@ -4031,8 +4031,8 @@
       <xdr:row>27</xdr:row>
       <xdr:rowOff>24660</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId28">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="76" name="Entrada de lápiz 75">
@@ -4051,7 +4051,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="76" name="Entrada de lápiz 75">
@@ -4096,8 +4096,8 @@
       <xdr:row>40</xdr:row>
       <xdr:rowOff>130320</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId30">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="88" name="Entrada de lápiz 87">
@@ -4116,7 +4116,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="88" name="Entrada de lápiz 87">
@@ -4161,8 +4161,8 @@
       <xdr:row>50</xdr:row>
       <xdr:rowOff>20400</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId32">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="96" name="Entrada de lápiz 95">
@@ -4181,7 +4181,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="96" name="Entrada de lápiz 95">
@@ -4226,8 +4226,8 @@
       <xdr:row>49</xdr:row>
       <xdr:rowOff>119460</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId34">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="97" name="Entrada de lápiz 96">
@@ -4246,7 +4246,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="97" name="Entrada de lápiz 96">
@@ -4291,8 +4291,8 @@
       <xdr:row>68</xdr:row>
       <xdr:rowOff>142440</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId36">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="100" name="Entrada de lápiz 99">
@@ -4311,7 +4311,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="100" name="Entrada de lápiz 99">
@@ -4356,8 +4356,8 @@
       <xdr:row>67</xdr:row>
       <xdr:rowOff>152580</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId38">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="101" name="Entrada de lápiz 100">
@@ -4376,7 +4376,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="101" name="Entrada de lápiz 100">
@@ -4421,8 +4421,8 @@
       <xdr:row>62</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId40">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="104" name="Entrada de lápiz 103">
@@ -4441,7 +4441,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="104" name="Entrada de lápiz 103">
@@ -4486,8 +4486,8 @@
       <xdr:row>65</xdr:row>
       <xdr:rowOff>69900</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId42">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="105" name="Entrada de lápiz 104">
@@ -4506,7 +4506,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="105" name="Entrada de lápiz 104">
@@ -4551,8 +4551,8 @@
       <xdr:row>49</xdr:row>
       <xdr:rowOff>100740</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId44">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="108" name="Entrada de lápiz 107">
@@ -4571,7 +4571,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="108" name="Entrada de lápiz 107">
@@ -4616,8 +4616,8 @@
       <xdr:row>35</xdr:row>
       <xdr:rowOff>82200</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId46">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="109" name="Entrada de lápiz 108">
@@ -4636,7 +4636,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="109" name="Entrada de lápiz 108">
@@ -4681,8 +4681,8 @@
       <xdr:row>35</xdr:row>
       <xdr:rowOff>162120</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId48">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="110" name="Entrada de lápiz 109">
@@ -4701,7 +4701,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="110" name="Entrada de lápiz 109">
@@ -4746,8 +4746,8 @@
       <xdr:row>36</xdr:row>
       <xdr:rowOff>28500</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId50">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="111" name="Entrada de lápiz 110">
@@ -4766,7 +4766,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="111" name="Entrada de lápiz 110">
@@ -4811,8 +4811,8 @@
       <xdr:row>66</xdr:row>
       <xdr:rowOff>140520</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId52">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="112" name="Entrada de lápiz 111">
@@ -4831,7 +4831,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="112" name="Entrada de lápiz 111">
@@ -4876,8 +4876,8 @@
       <xdr:row>83</xdr:row>
       <xdr:rowOff>101460</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId54">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="126" name="Entrada de lápiz 125">
@@ -4896,7 +4896,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="126" name="Entrada de lápiz 125">
@@ -4941,8 +4941,8 @@
       <xdr:row>20</xdr:row>
       <xdr:rowOff>79380</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId56">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="131" name="Entrada de lápiz 130">
@@ -4961,7 +4961,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="131" name="Entrada de lápiz 130">
@@ -5050,8 +5050,8 @@
       <xdr:row>29</xdr:row>
       <xdr:rowOff>74580</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId59">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="140" name="Entrada de lápiz 139">
@@ -5070,7 +5070,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="140" name="Entrada de lápiz 139">
@@ -5115,8 +5115,8 @@
       <xdr:row>31</xdr:row>
       <xdr:rowOff>34140</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId61">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="141" name="Entrada de lápiz 140">
@@ -5135,7 +5135,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="141" name="Entrada de lápiz 140">
@@ -5180,8 +5180,8 @@
       <xdr:row>30</xdr:row>
       <xdr:rowOff>104400</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId63">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="147" name="Entrada de lápiz 146">
@@ -5200,7 +5200,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="147" name="Entrada de lápiz 146">
@@ -5245,8 +5245,8 @@
       <xdr:row>30</xdr:row>
       <xdr:rowOff>85320</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId65">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="152" name="Entrada de lápiz 151">
@@ -5265,7 +5265,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="152" name="Entrada de lápiz 151">
@@ -5346,8 +5346,8 @@
       <xdr:row>33</xdr:row>
       <xdr:rowOff>74760</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId68">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="156" name="Entrada de lápiz 155">
@@ -5366,7 +5366,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="156" name="Entrada de lápiz 155">
@@ -5416,8 +5416,8 @@
       <xdr:row>8</xdr:row>
       <xdr:rowOff>80880</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="15" name="Entrada de lápiz 14">
@@ -5436,7 +5436,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="15" name="Entrada de lápiz 14">
@@ -5481,8 +5481,8 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>9540</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="16" name="Entrada de lápiz 15">
@@ -5501,7 +5501,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="16" name="Entrada de lápiz 15">
@@ -5589,17 +5589,17 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">218 480,'-5'1,"1"0,0 0,-1 0,1 0,0 1,0 0,0-1,0 2,0-1,1 0,-1 1,0-1,1 1,0 0,0 0,0 1,0-1,0 1,1-1,0 1,-3 4,-7 14,1 0,-13 35,18-40,-2 2,-51 147,54-148,1 1,1-1,0 1,2-1,0 1,1 0,3 26,-2-40,1 0,-1 1,1-1,0 0,1-1,-1 1,1 0,0-1,0 1,0-1,1 0,-1 0,1 0,0-1,1 1,-1-1,0 0,1 0,0 0,-1-1,7 2,14 6,0-1,1-1,30 5,-12-3,-4 0,13 5,1-2,1-2,0-3,72 2,-125-10,1 0,-1-1,1 1,0-1,-1 1,1-1,-1 0,0 0,1 0,-1 0,0 0,0-1,1 1,-1-1,0 0,0 1,-1-1,1 0,0 0,-1 0,1 0,-1 0,1-1,-1 1,0 0,0-1,0 1,0-1,-1 1,1-1,-1 1,1-4,1-10,-1 0,0 0,-1 0,-3-19,1 13,0-45,1 17,-9-57,8 93,-1-1,0 2,-1-1,-1 0,0 1,-1 0,0 0,-14-20,14 25,0 1,-1 0,0 0,-1 0,1 1,-1 0,0 1,-1 0,1 0,-1 0,0 1,0 1,-15-4,-10-1,0 1,-52-2,33 4,16 1,5 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1224.99">986 559,'-2'1,"0"0,0 0,0 0,0 0,0 0,0 1,1-1,-1 1,0-1,1 1,-1-1,1 1,0 0,-1-1,1 1,0 0,-1 4,-19 37,21-42,-8 21,1 1,1 1,1-1,1 1,-2 46,13 123,-5-178,0 0,1-1,1 1,1-1,0 0,1 0,0 0,1-1,0 0,2 0,-1-1,1 0,17 17,-2-6,0-1,2-2,0 0,1-2,34 17,-43-24</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2562.99">1356 1194,'0'-4,"1"-1,1 1,-1 0,1 0,-1-1,1 1,0 0,1 0,-1 0,1 1,0-1,-1 1,2-1,-1 1,0 0,1 0,-1 0,5-2,9-7,0 1,29-13,-31 16,1 2,0 0,0 0,1 2,-1 0,1 1,28-2,-40 4,0 1,0 0,0 1,0-1,0 1,1 0,-1 0,-1 0,1 1,0 0,0 0,0 0,-1 1,0-1,1 1,-1 0,0 0,0 1,0-1,-1 1,1 0,-1 0,0 0,0 0,0 0,-1 1,0-1,0 1,3 6,0 14,0 0,-2 0,0 0,-2 0,-3 47,1-26,-1-22,0 1,-2 0,-1-1,0 0,-2 0,-1 0,-1-1,-23 42,17-37,-2-1,-1-1,-2-1,0 0,-1-1,-41 33,46-43,0-1,-1-1,-1-1,-33 17,47-26,0-1,0 1,0-1,-1 0,1-1,0 1,0 0,0-1,-1 0,1 0,0-1,0 1,-5-2,6 1,0 0,0-1,0 1,1-1,-1 1,0-1,1 0,0 0,-1-1,1 1,0 0,0-1,0 1,0-1,1 0,-1 1,1-1,0 0,-1 0,0-3,0-1,0-1,0 1,1 0,0 0,0 0,1-1,0 1,0 0,0-1,1 1,0 0,1 0,0-1,0 1,0 1,1-1,0 0,0 0,1 1,-1 0,1 0,1 0,-1 0,1 1,0-1,1 1,-1 0,1 1,0 0,0 0,0 0,1 0,-1 1,1 0,0 1,0-1,0 1,0 0,0 1,1 0,6 0,9 0,-1 1,1 1,0 1,-1 1,0 1,0 0,0 2,0 1,-1 1,0 0,-1 2,30 18,38 27,-64-41</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3462">1806 744,'10'-5,"-1"-1,1-1,-1 0,9-8,-10 7,0 1,1 0,0 1,1 0,11-6,14-4,-15 6,0 1,0 1,42-10,-55 17,1 0,-1 0,1 1,-1 0,1 0,-1 1,0 0,1 0,-1 0,0 1,0 1,0-1,0 1,0 0,12 8,14 12,-1 1,-1 2,52 56,71 105,32 34,-181-215,0-1,0 0,1 0,-1 0,1-1,1 1,-1-1,0-1,1 1,0-1,-1-1,15 5,1-6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4260">2970 480,'-16'1,"1"0,0 1,0 0,0 2,0-1,0 2,1 0,-1 1,2 0,-1 1,1 0,0 2,0-1,1 1,0 1,0 0,-14 18,-9 15,1 1,2 2,-37 74,12-22,43-79,-1-1,-1 0,-1-1,0-1,-1-1,-1 0,-35 21,2 0,28-20,5-6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5010.99">3129 1115,'4'0,"2"5,0 5,-2 15,-1 8,-1 12,-1 2,0-2,3-9,2-5,4-9,1-8</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5401">3155 797,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6953.99">3129 4,'45'-1,"-27"-1,-1 2,1 0,0 0,26 6,-40-5,0 0,0 0,0 0,0 1,-1-1,1 1,-1 0,1 0,-1 1,1-1,-1 0,0 1,0 0,0 0,-1 0,1 0,-1 0,0 1,0-1,0 1,0 0,0-1,-1 1,2 6,3 25,-2-1,-2 1,-1 0,-1 0,-8 45,7-66,1-10,0 0,-1 1,1-1,-1 0,0 0,0 1,-1-1,1 0,-1 0,0-1,0 1,0 0,-1 0,1-1,-1 0,0 1,0-1,0 0,-4 3,3-5,1 1,0-1,-1 0,1 0,-1 0,1 0,-1 0,1-1,-1 0,0 1,1-2,-1 1,1 0,-1-1,0 1,1-1,-1 0,1 0,0 0,-1-1,1 1,0-1,-4-2,4 2,0 1,1-1,0 1,-1-1,1 0,0 0,0 0,0 0,0 0,0 0,0-1,0 1,1-1,-1 1,1-1,0 1,0-1,0 0,0 0,0 0,0-4,1 1,0 1,1 0,-1 0,1 0,1 0,-1-1,0 2,1-1,0 0,0 0,5-6,1-2,1 0,0 1,1 0,1 0,-1 1,2 1,17-14,-22 20,-1 0,1 1,-1-1,1 1,0 0,0 1,0 0,1 0,-1 0,0 1,1 0,-1 1,1 0,-1 0,1 0,-1 1,1 0,8 3,7 3,-1 2,-1 0,1 2,27 17,-24-13,0-1,29 10,-28-15</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8287.99">3975 533,'4'0,"2"-4,9-2,29-5,38 1,37-4,25 2,6 2,4 2,4 4,-3 2,-15 1,-26 1,-23 0,-28 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8826">3817 1141,'4'0,"15"0,32 0,11 0,4 0,0 0,-2 0,1 0,8 0,1 0,0 0,2 5,-8 1,-6 4,0 6,-11-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10412">6462 321,'-36'0,"0"1,-54 10,76-8,-1 1,0 0,1 1,0 1,0 0,1 1,0 1,-21 15,-13 14,1 2,3 2,-73 89,107-116,0 2,1-1,1 1,0 0,1 1,1-1,1 1,0 0,1 1,-1 26,0-10,-11 42,4-39,5-19,1 1,0-1,2 1,0-1,0 21,3-34,0 1,1-1,0 0,0 0,0 0,0 0,1 0,0 0,0 0,0 0,1 0,0-1,0 0,0 1,0-1,0 0,1 0,0-1,0 1,0-1,0 0,9 5,10 3,1 0,0-2,0-1,1 0,0-2,0-1,1-1,-1-1,1-2,48-2,-64-1,0 1,0-2,-1 0,1 0,-1 0,0-1,0-1,0 1,0-2,-1 1,0-1,0 0,0-1,-1 0,0 0,0 0,9-15,0-2,0 0,-2-2,-1 1,19-54,-22 48,-2-1,0 1,4-65,-8-98,-5 183,0-1,-1 1,0-1,-1 1,-1 0,0 0,0 0,-1 0,0 1,-1 0,-13-19,13 21,0 1,-1-1,0 1,0 0,0 0,-1 1,0 0,0 1,0-1,-1 2,0-1,0 1,0 0,-13-2,0 2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">227 459,'-6'1,"2"0,0 0,-1 0,1 0,0 1,-1 0,1-1,0 2,0-1,1-1,-1 2,-1-1,2 1,0 0,0 0,0 1,0-1,0 0,1 0,0 1,-4 4,-6 13,0 0,-12 33,17-37,-1 1,-53 141,55-142,2 1,1-1,0 1,2 0,0 0,1 0,3 25,-2-38,1 0,-1 0,1 0,0 0,2-1,-2 1,1-1,0 0,0 1,0-1,1 0,-1-1,2 1,-1-1,1 1,-1-1,0 0,1 0,1-1,-2 0,7 2,15 6,0-2,1 0,31 4,-12-2,-4 0,13 4,1-2,1-1,0-4,75 3,-130-10,1 0,0-1,0 1,0-1,-1 1,1-1,-1 0,0 0,1 0,-1 0,0 0,1-1,0 2,-1-2,0 0,0 1,-1-1,1 0,0 0,-1 0,1 0,-1 0,1-1,-1 1,0 1,0-2,0 1,1-1,-2 1,1-1,-1 1,1-4,1-9,-1 0,0 0,-1-1,-3-17,1 12,-1-43,2 16,-9-55,8 90,-1-1,0 1,-1 0,-2-1,1 2,-1 0,0-1,-15-18,15 23,-1 1,0 1,0-1,-1 0,0 1,0 1,0 0,-2 0,2 0,-1 1,-1 0,1 1,-16-4,-10 0,-1 0,-53-2,34 4,16 2,6 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1224.99">1025 535,'-2'1,"0"0,0 0,0 0,-1 0,1 0,0 0,1 0,-1 1,0-1,1 1,-1-1,1 1,0 0,-1-1,1 1,0 0,-1 4,-20 35,22-40,-8 20,0 1,2 1,1-1,1 1,-3 44,15 117,-6-169,0-1,1-1,1 2,1-2,1 0,0 1,0-1,1 0,1-1,1 0,-1 0,2-1,17 17,-2-6,0-1,2-2,0 0,1-1,35 15,-44-22</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2562.99">1409 1142,'0'-4,"2"0,0 0,-1 0,1 0,-1-1,1 2,0-1,1 0,-1 0,1 1,0-1,-1 2,3-2,-2 1,0 0,1 0,-1 0,5-2,10-6,0 0,30-12,-33 16,2 1,-1 0,1 1,1 1,-2 0,2 1,29-2,-42 4,0 1,0 0,1 1,-1-1,0 1,1 0,-1 0,0 0,0 1,0 0,0 0,0 0,0 1,-1-1,1 0,-1 1,0 0,0 1,1-1,-2 1,1 0,-1-1,0 1,0 0,0 0,-1 1,0-2,0 2,4 6,-1 13,0 0,-2-1,0 1,-2 0,-3 45,1-25,-1-21,0 1,-2 0,-1-1,0 0,-3 0,0 0,-1-1,-25 40,19-35,-3-1,-1-2,-1 0,-1 0,-1-1,-43 32,49-42,-1 0,0-2,-2 0,-34 15,49-24,0-1,-1 1,1-1,-1 0,1-1,0 1,0 0,-1-1,0 0,1 0,0-1,0 1,-6-2,7 1,0 0,0-1,0 1,1-1,-1 2,0-2,0 0,1 0,-1-1,1 1,0 0,0-1,0 1,0-1,1 1,-1 0,1-1,0 0,-1 0,0-3,-1 0,1-2,0 1,1 1,0-1,0 0,1 0,0 0,0 0,0-1,1 2,0-1,1 0,0 0,0 0,1 1,0 0,0-1,0 0,1 1,-1 1,1-1,2 0,-2 0,1 2,0-2,1 1,0 0,0 2,0-1,0 0,0 0,2 0,-2 1,1 1,1 0,-1-1,0 1,0 0,1 1,0 0,7 0,8 0,0 1,1 1,0 1,-1 1,0 1,0-1,0 3,-1 1,0 1,0-1,-1 3,31 17,39 25,-66-38</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3462">1877 712,'11'-5,"-2"-1,1 0,0-1,8-7,-9 6,-1 1,1 0,1 2,0-1,12-5,14-5,-15 7,0 0,0 1,43-9,-57 16,2 0,-2 0,1 1,0 0,0 0,-1 1,1 0,0 0,-1 0,0 1,1 1,-1-1,0 1,0 0,13 7,15 12,-2 1,-1 2,54 53,74 101,34 33,-189-207,0 0,0 0,2 0,-2 0,1-2,1 2,0-1,-1-1,1 1,0-1,0-2,14 6,2-6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4260">3087 459,'-16'1,"0"0,0 1,1 0,-1 2,1-1,-1 1,1 1,0 1,1 0,0 0,0 1,1 2,-1-2,2 2,-1 1,1-1,-15 18,-10 14,2 1,2 2,-39 71,13-21,44-76,0-1,-2 0,-1 0,1-2,-2-1,-1 1,-36 19,2 0,29-18,5-7</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5010.99">3252 1067,'5'0,"1"4,0 6,-2 14,-1 8,-1 11,-1 2,1-2,2-9,2-4,4-9,2-8</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5401">3279 762,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6953.99">3252 4,'47'-1,"-28"-1,-1 2,0 0,1 0,27 6,-42-5,0 0,0 0,0 0,1 0,-2 0,1 1,-1 0,1 0,-1 1,1-1,-1 0,1 1,-1 0,0-1,-1 1,1 0,-1 0,0 1,0-1,0 1,0-1,1 0,-2 1,2 6,3 23,-2 0,-2 0,-1 1,-1-1,-8 44,7-64,1-9,0 0,-1 1,1-2,-1 1,0 0,0 1,-1-1,1-1,-2 1,1-1,0 1,0 0,-1 0,1-2,-1 1,0 1,0-1,0 0,-5 3,4-5,1 1,0-2,-1 1,1 0,-2 0,2 0,-1 0,1-1,-1 0,0 1,1-2,-2 1,2 0,-1-1,0 1,1-1,-1 0,1 0,0 0,-2 0,2 0,0-1,-4-2,4 2,0 1,1-1,-1 1,0-1,1 0,0 0,0 0,0 1,0-1,0 0,0-1,0 1,1-1,-1 1,1-1,0 1,-1 0,1-1,0 0,0 0,0-4,1 1,0 2,1-1,-1 0,1 0,1 1,0-2,-1 2,1-1,0 0,0 1,5-7,1-1,2-1,-1 2,1-1,2 1,-2 0,3 2,17-14,-23 19,-1 0,2 1,-2-1,1 2,1-1,-1 1,0 0,1 0,0 0,-1 1,1 0,0 1,0 0,-1 0,1 0,0 1,0 0,9 3,7 3,-2 1,0 1,1 1,28 17,-25-13,0 0,30 9,-29-15</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8287.99">4132 510,'4'0,"2"-4,10-2,30-4,39 0,38-3,27 1,6 3,4 1,4 4,-2 2,-17 1,-26 1,-25 0,-28 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8826">3968 1092,'4'0,"15"0,35 0,10 0,5 0,-1 0,-1 0,0 0,9 0,1 0,0 0,2 4,-8 2,-7 4,1 5,-12-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10412">6717 307,'-37'0,"-1"1,-55 10,78-9,-1 2,1 0,0 1,1 1,-1-1,2 2,-1 1,-21 14,-14 13,1 2,3 3,-75 84,111-111,-1 3,2-2,1 1,-1 1,2 0,1-1,1 2,0-1,0 1,0 25,0-9,-11 39,3-36,6-19,1 1,-1-1,3 2,0-2,0 20,3-32,0 1,1-2,0 1,0 0,0 0,0-1,1 1,0 0,1 0,-1 0,1-1,0 0,0 0,0 1,0-1,0-1,1 1,1-1,-1 1,0-1,0 0,10 4,10 4,0-1,1-1,0-1,1-1,0-1,0-1,1-1,-1-1,1-2,50-2,-66-1,-1 1,0-2,0 0,0 0,0 0,-1-1,0 0,1 0,-1-2,-1 1,1 0,-1-1,0-1,0 0,-1 1,0-1,10-14,-1-2,1 0,-2-2,-2 1,20-51,-22 45,-3-1,0 2,5-63,-9-94,-5 176,0-2,-1 2,0-2,-1 2,-2-1,1 1,0-1,-1 1,0 0,-1 1,-14-19,14 20,-1 1,0 0,0 0,-1 0,1 1,-1 0,0 0,-1 1,1 0,-1 1,-1-1,1 1,-1 0,-12-1,-1 1</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -5626,11 +5626,11 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">54 75,'18'-1,"0"-1,0-1,0 0,31-11,21-5,17 5,0 4,0 4,1 4,153 15,-178-10,29 3,-84-5,1 0,-1 1,0 0,0 1,0-1,0 2,0-1,7 5,6 8</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1340">1 49,'103'6,"0"3,103 25,-55-9,-96-15,-1 2,53 20,-106-32,0 1,0-1,-1 0,1 0,0 0,0 0,-1 0,1 1,0-1,0 0,-1 1,1-1,0 0,-1 1,1-1,-1 1,1-1,-1 1,1 0,0-1,-1 1,0-1,1 1,-1 0,1-1,-1 1,0 0,0 0,1-1,-1 1,0 0,0 0,0-1,0 1,0 0,0 0,0-1,0 1,0 0,0 0,0-1,0 1,-1 0,1 0,0-1,0 1,-1 0,1-1,-1 1,1 0,-1-1,1 1,-1-1,0 2,-41 33,30-26,-116 92,4 5,6 6,-113 135,222-236,1-2,1-1,-1 2,1-1,1 1,0 0,-8 18,14-27,0 0,-1 0,1 0,0 0,0 0,-1 0,1 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,1 0,-1 0,1-1,-1 1,1 0,-1 0,1 0,-1 0,1 0,0-1,-1 1,1 0,0-1,1 2,33 9,32-4,0-3,0-2,87-11,-32 3,-120 6,53-3,0 3,75 10,-94-4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2876.99">1933 578,'-49'0,"10"-2,0 3,-52 6,82-6,1 1,-1 0,0 0,1 0,0 1,0 1,-1-1,2 1,-1 1,0-1,1 1,0 0,0 1,1 0,-12 13,14-12,0 1,0 0,0 0,1 0,1 1,-1-1,2 1,-1-1,1 1,0 0,1-1,0 1,1 14,0-13,0 0,1 0,0 0,1 0,0-1,0 1,1-1,0 0,0 0,1 0,10 12,-4-9,1-1,0-1,0 0,1-1,1 0,0-1,0 0,0-1,21 6,-3-2,0-2,1-1,48 5,-77-12,0 0,0-1,0 0,0 0,0 0,0 0,0-1,0 1,0-1,0 0,0 0,-1-1,1 1,0-1,3-2,-4 2,-1 0,0-1,0 1,0-1,0 0,0 0,-1 0,1 0,-1 0,0 0,1 0,-2 0,1 0,0 0,-1-1,1 1,-1 0,0-1,0-2,2-28,-2 0,-1 1,-2-1,-1 1,-10-41,11 65,1 0,-2 0,1 0,-1 1,-1 0,1 0,-1 0,-1 0,1 1,-1 0,-1 0,1 0,-1 1,0 0,-1 1,1-1,-1 1,0 1,0-1,-1 1,0 1,1 0,-17-4,-6 2,5 3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3934.99">1933 366,'-2'151,"4"163,-1-307,1 0,-1-1,1 1,0 0,0-1,1 0,0 1,0-1,1 0,0-1,0 1,0 0,0-1,1 0,0 0,0-1,0 1,9 4,10 7,1-1,54 23,-66-32,59 18,-38-17</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6500.99">3308 419,'4'-4,"11"-2,12 1,10 0,8 2,1 1,-3 1,-5 0,-3 1,-9 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">56 72,'19'-1,"0"-1,0-1,0 0,32-10,22-5,19 4,-1 5,0 3,1 4,160 14,-186-9,30 3,-87-5,0 0,0 1,-1 0,0 1,1-1,-1 2,0-2,8 6,6 7</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1340">1 47,'108'6,"0"2,107 25,-57-9,-100-14,-1 1,55 20,-111-31,0 1,0-1,-1 0,1 0,0 0,0 0,-1 0,1 1,0-1,0 0,-1 1,1-1,0 0,-1 1,1-1,-1 1,1-1,-1 1,1 0,0-1,-1 1,0-1,1 1,-1 0,1-1,-1 1,0 0,0-1,1 0,-1 1,0 0,0 0,0-1,0 1,0 0,0 0,0-1,0 1,0 0,0 0,0-1,0 1,-1 0,1 0,0-1,0 1,-1 0,1-1,-1 1,1 0,-1-1,1 1,-1-1,0 2,-43 31,32-24,-122 88,4 5,6 5,-118 130,233-226,1-2,0-2,0 3,1-1,0 0,1 1,-9 17,15-26,0 0,-1-1,1 1,0 0,0 0,-1 0,1 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,1 0,-1 0,1-1,-1 1,1 0,-1 0,1 0,-1 0,2 0,-1-1,-1 1,1 0,0-1,1 1,34 10,35-4,-1-3,0-2,91-11,-33 3,-126 6,55-3,1 3,78 10,-98-4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2876.99">2024 555,'-52'0,"12"-2,-1 3,-55 6,87-6,1 1,-2 0,1-1,0 1,1 1,0 1,-2-1,3 1,-1 1,-1-2,2 2,-1 0,1 1,1 0,-13 12,15-11,0 0,-1 1,1 0,1-1,1 2,-1-1,2 0,-1 0,1 1,0-1,1 0,0 1,1 13,0-13,0 1,1-1,0 1,1 0,0-2,0 2,2-1,-1-1,0 1,1-1,11 13,-5-10,2 0,0-2,-1 1,2-1,0-1,1 0,0 0,-1-2,23 7,-4-3,1-1,1-1,49 4,-79-11,-1 0,0-1,0 0,0 0,0 0,1 0,-1-1,0 1,0-1,0 0,1 0,-2-1,1 1,0-1,3-1,-3 1,-2 0,0-1,0 1,0-1,0 0,0 0,-1 0,1 1,-1-1,0 0,1 0,-2 0,2 0,-1 0,-1-1,1 2,-1-1,0-1,0-2,2-27,-2 1,-1 0,-2-1,-2 2,-9-40,11 62,0 0,-1 1,1-1,-1 1,-1 1,1-1,-2 0,0 1,1 0,-2 0,0 1,1-1,-1 1,-1 0,0 1,1 0,-2 0,1 1,-1-1,0 1,0 2,0-1,-17-4,-6 2,4 3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3934.99">2024 351,'-2'145,"4"157,-1-295,1-1,-1 0,1 1,0 0,0-2,1 1,0 1,1-1,0-1,0 0,0 1,0 0,0-2,2 1,-1 0,0-1,0 1,10 3,10 8,1-2,57 23,-69-32,61 18,-39-16</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6500.99">3463 402,'4'-3,"12"-3,12 1,11 0,8 2,1 1,-3 1,-5 0,-3 1,-10 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -5717,16 +5717,16 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1615 185,'4'0,"11"0,21 0,17 0,5 0,6 0,5 0,27 0,7 0,-6 0,-2 0,-11 0,-12 0,-9 5,-15 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-1337.97">319 476,'4'5,"2"42,-1 48,0 31,-2 26,-1 5,-1-11,0-30</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-756">1 979,'0'-1,"0"0,1 1,-1-1,0 0,1 0,-1 0,1 0,0 0,-1 0,1 1,0-1,-1 0,1 1,0-1,0 0,-1 1,1-1,0 1,0-1,0 1,0 0,0-1,0 1,0 0,2-1,32-6,-27 6,126-15,1 6,151 8,-185 2,-80 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2123">1271 238,'24'0,"0"-1,1 1,0 2,-1 0,1 1,43 12,-59-12,269 99,-233-83,-1 3,-1 1,79 58,-105-69,0-1,34 16,-1 0,-48-26,-1-1,0 0,0 1,0-1,0 1,0-1,-1 1,1 0,0 0,0-1,0 1,0 0,-1 0,1 0,0 0,-1-1,1 1,-1 0,1 0,-1 0,1 0,-1 1,0-1,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 1,0-1,-1 0,0 2,-2 1,0 1,0-1,-1 0,1 0,-1 0,0 0,-6 4,-23 18,-1-1,-60 33,-333 148,118-61,266-121,42-24,1 0,0 0,-1 0,1 0,0 0,0 1,-1-1,1 0,0 0,-1 0,1 0,0 0,0 1,-1-1,1 0,0 0,0 0,0 1,-1-1,1 0,0 0,0 1,0-1,0 0,0 0,-1 1,1-1,0 0,0 1,0-1,0 0,0 1,0-1,0 0,0 0,0 1,0-1,0 0,0 1,0-1,0 0,1 1,15 2,35-5,-44 1,14-1,152-7,-146 10,0 0,-1 2,1 1,39 11,-63-14,67 20,108 47,-79-25,-56-28</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3698">2859 794,'-35'0,"1"1,-1 2,-45 9,67-9,0 1,0 0,1 1,-1 1,1 0,0 0,0 1,1 1,0 0,1 0,-15 16,-9 10,2 2,1 1,3 1,0 1,-35 71,60-103,0 1,0-1,0 1,1 0,1 0,-1 0,1 0,1 0,-1 0,2 0,-1 0,1 0,0 0,0 0,5 14,-4-17,0-1,1 1,0 0,0-1,0 0,0 0,0 0,1 0,0 0,0 0,0-1,0 0,0 0,1 0,-1-1,1 1,0-1,0 0,0 0,0-1,0 1,0-1,0 0,10 0,51 1,99-10,-146 7,-9-1,0 0,0 0,0-1,0-1,0 0,0 0,-1-1,0 0,0 0,-1-1,1 0,-1-1,0 0,-1 0,0-1,9-11,10-15,-2-2,31-57,-55 92,11-18,0-1,-1 0,-2-1,0 0,-1 0,-1-1,-1 0,-1 1,2-43,-5 46,-3-54,1 69,1 0,-1 0,1 0,-1 0,0 0,0 0,0 1,-1-1,1 0,-1 0,1 1,-1-1,0 1,0-1,0 1,0 0,0 0,-1 0,-3-2,5 3,0 1,-1-1,1 1,-1 0,1 0,0-1,-1 1,1 0,-1 0,1 0,-1 1,1-1,0 0,-1 0,1 1,0-1,-1 1,1-1,0 1,-1 0,1-1,0 1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 1,0-1,1 0,-1 0,0 3,-22 51,22-53,-25 88,-27 187,49-251,0-3,1 1,2 0,0-1,2 25,-1-43,1-1,-1 1,1-1,0 1,0-1,0 0,1 0,0 1,-1-1,2 0,-1 0,0-1,1 1,-1 0,1-1,0 0,1 1,-1-1,0 0,1-1,-1 1,1-1,0 1,0-1,0 0,0-1,6 3,14 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4802.03">3176 1243,'0'-3,"1"-1,0 0,0 0,0 0,1 1,-1-1,1 1,0-1,0 1,0 0,1-1,-1 1,1 0,-1 1,1-1,0 0,5-2,-7 3,1 1,0-1,0 1,0 0,0 0,0-1,0 1,0 1,0-1,0 0,0 0,1 1,-1 0,0-1,0 1,1 0,-1 0,0 0,0 0,1 0,-1 1,0-1,0 1,1-1,-1 1,0 0,0 0,0 0,0 0,0 0,2 3,1 2,0 0,0 0,0 1,-1 0,0 0,-1 0,0 0,0 0,3 13,14 76,-17-81,4 31,-1 0,-3 1,-4 84,0-124,0 0,-1-1,-1 1,1-1,-1 1,0-1,0 0,-1 0,1 0,-1-1,-1 0,1 1,-1-1,0-1,0 1,0-1,-1 0,0 0,0 0,-11 5,-14 5,0-1,-64 18,74-25,14-4,-7 2,0 0,0-1,0 0,0-1,-16 0,28-2,0 0,0 0,0 0,0 0,0-1,0 1,0-1,0 0,0 1,1-1,-1 0,0 0,0 0,1 0,-1 0,1-1,-1 1,-1-2,2 0,0 1,0 0,0-1,0 1,0 0,1-1,-1 1,1-1,0 1,0-1,-1 1,2-1,-1 0,0 1,1-1,-1 1,1 0,1-4,0-1,0 0,1 1,0-1,0 1,1 0,0 0,0 0,0 1,0-1,1 1,0 0,0 0,1 1,-1-1,1 1,0 1,0-1,1 1,-1 0,0 0,1 1,0 0,0 0,0 0,-1 1,1 0,11 0,-2 0,1 1,0 1,-1 0,1 1,-1 0,0 2,0 0,0 1,0 0,25 13,1 6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5682">4129 582,'4'0,"11"-4,21-6,21-7,16 1,-5 7,-10 19,-5 20,-3 33,-6 19,-5 9,-5 3,-9-6,-3-13,-2-11,-4-11,5-7,-2-10</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6235">4896 529,'-9'0,"-12"0,-16 18,-33 24,-23 23,-18 14,-43 38,-24 13,10-11,29-21,38-24,41-23,30-21</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7026">5240 1058,'0'23,"0"25,0 13,-5 6,-1 0,1-11</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8493">5267 0,'3'1,"0"-1,0 1,1 0,-1-1,0 1,0 1,0-1,0 0,0 1,0 0,0-1,0 1,-1 0,1 0,-1 1,1-1,-1 1,0-1,0 1,0 0,0-1,-1 1,1 0,-1 0,0 0,1 0,-2 1,1-1,0 0,0 5,3 13,-1 1,0 0,-2 31,-1-37,1 23,1 1,-8 82,5-111,-1 0,0 0,-1 0,0 0,-1-1,0 1,-1-1,0 0,-1 0,0-1,0 0,-9 10,1-3,-34 32,45-46,1 0,0 0,-1 0,0-1,1 1,-1-1,0 1,0-1,0 0,0 0,0-1,0 1,0-1,0 1,0-1,0 0,0 0,-3 0,3-1,1-1,0 1,0 0,0 0,0-1,0 1,1-1,-1 0,0 1,1-1,-1 0,1 0,-1 0,1 0,0 0,0 0,0 0,0-1,0 1,1 0,-1-1,1 1,-1 0,1-1,0-4,-1-6,0 0,1 0,2-17,-1 28,0-1,-1 1,1 0,0-1,0 1,0 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,0 0,0 1,0-1,0 1,0 0,0-1,0 1,1 0,2-1,58-16,-52 16,40-8,2 2,-1 2,0 3,86 6,-127-2,0 0,-1 1,1 1,18 6,-2 3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1664 176,'4'0,"11"0,22 0,18 0,5 0,5 0,7 0,26 0,8 0,-6 0,-2 0,-11 0,-13 0,-9 5,-16 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-1337.97">329 454,'4'5,"2"40,-1 45,0 30,-2 25,-1 5,-1-11,0-28</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-756">1 934,'0'-1,"0"0,1 1,-1-1,0 0,1 0,-1 0,1 0,0 0,-1 0,1 1,0-1,-1 0,1 1,0-1,0 0,-1 1,1-1,0 1,0 0,0 0,0 0,0-1,0 1,1 0,1-1,33-6,-28 6,130-14,1 5,156 8,-191 2,-83 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2123">1309 227,'25'0,"0"-1,0 1,1 2,-1 0,1 1,44 11,-61-11,277 94,-239-79,-2 3,-1 1,82 56,-109-67,1-1,34 16,0 0,-50-25,-1-1,0 0,0 1,0-1,0 1,0-1,-1 1,1 0,0 0,0-1,0 1,0 0,-1 0,1 0,0-1,-1 0,1 1,-1 0,1 0,-1 0,2 0,-2 1,0-1,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 1,0-1,-1 0,-1 1,-1 2,0 1,0-1,-1 0,1-1,-1 1,0 0,-7 4,-23 16,-1 0,-61 32,-344 140,121-58,275-115,43-23,1 0,0 0,-1 0,1 0,0 0,0 1,-1-1,1 0,0 0,-1 0,1 0,0 0,0 1,-1-1,1 0,0 0,0 0,0 1,-1-1,1 0,0 0,0 1,0-1,0 0,0 0,-1 1,1-1,0 0,0 1,0-1,0 0,0 1,0-1,0 0,0 0,0 1,0-1,0 0,0 1,0-1,0 0,1 1,15 2,37-5,-46 1,15-1,156-7,-150 10,0 0,-2 2,2 1,40 10,-65-13,69 19,112 45,-82-24,-58-27</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3698">2945 757,'-36'0,"1"1,-1 2,-47 9,70-9,0 0,-1 1,2 1,-2 1,2-1,0 1,-1 1,2 0,0 1,0 0,-14 15,-10 9,2 2,1 2,3 0,0 1,-36 68,62-98,0 0,0 0,0 1,1-1,1 1,-1-1,1 1,1 0,-1-1,2 1,-1 0,1-1,0 1,0 0,5 13,-4-17,0 0,1 1,0 0,0-2,0 1,0 0,1 0,0 0,0 0,0-1,0 0,0 0,0 0,1 0,0-1,0 1,0-2,0 1,0 0,0-1,0 1,1-1,-1 0,10 0,53 1,102-10,-150 7,-10-1,0 1,1-1,-1-1,0-1,1 0,-1 0,-1 0,0-1,1 0,-2-1,1 1,-1-2,1 0,-2 1,0-2,10-10,9-15,-1-1,32-55,-57 88,11-17,0-1,0 0,-3-1,0 0,-1 0,0-1,-2 0,-1 1,2-41,-5 44,-3-52,1 66,1 0,-1 0,1 1,-1-1,0 0,0 0,0 1,-1-1,1 0,-1 1,1 0,-1-1,-1 1,1-1,0 1,0 0,0 0,-1 0,-3-1,5 2,0 1,-1-1,1 1,-1 0,1 0,0-1,-1 1,1 0,-1 0,1 0,-2 1,2-1,0 0,-1 0,1 1,0-1,-1 1,1-1,0 1,-1-1,1 0,0 1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 1,0-1,1 0,-1 0,0 3,-23 48,23-50,-26 84,-27 178,49-239,1-3,1 1,2 0,0-1,2 23,-1-40,1-1,-1 1,1-2,0 2,0-1,0 0,1 0,0 0,0 0,1 0,-1 0,0-1,1 1,-1-1,1 0,0 0,1 1,-1-1,0 0,1-1,0 0,0 0,0 1,0-1,0 0,0-1,6 3,15 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4802.03">3271 1186,'0'-3,"1"-1,1 0,-1 0,0 1,1 0,-1-1,1 1,0-1,0 1,0 0,1 0,-1 0,1 0,-1 1,1-1,0 0,6-1,-8 2,1 1,0-1,0 1,0 0,0 0,0-1,0 1,0 1,0-1,0 0,0 0,1 1,-1 0,1-1,-1 1,1 0,-1 0,0 0,0 0,1 0,-1 1,0-1,0 1,1-1,-1 1,0 0,0 0,0 0,1 0,-1 0,2 3,1 1,0 1,0 0,0 1,-1-1,1 1,-2 0,0-1,0 1,3 12,15 73,-18-78,4 30,-1 0,-3 0,-4 81,0-118,0 0,-1-2,-1 2,1-1,-1 1,0-2,0 1,-2 0,2-1,-1 0,-1 0,1 1,-1-2,0 0,0 1,-1-1,0 0,0 0,0-1,-12 6,-14 4,0 0,-65 16,75-23,15-4,-8 2,1 0,0-2,-1 1,1-1,-17 0,29-2,0 0,0 0,0 0,-1 0,1-1,0 1,0-1,0 0,0 1,1-1,-1 0,0 0,0 0,1 0,-1 0,1 0,-1 0,-1-2,2 0,0 1,0 0,0-1,0 1,0 0,1 0,-2 0,2-1,0 1,0-1,-1 1,2-1,-1 0,0 1,2 0,-2 0,1 0,1-4,0-1,0 1,1 0,0-1,0 2,1-1,0 0,0 0,0 2,1-2,0 1,0 0,0 1,1 0,-1-1,2 1,-1 1,0 0,1 0,-1 0,0 0,2 1,-1 0,0 0,0 0,0 1,0 0,11 0,-1 0,0 1,1 1,-2 0,2 1,-2 0,1 2,-1 0,1 1,-1-1,26 14,2 4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5682">4253 555,'4'0,"12"-4,21-5,21-7,18 0,-6 8,-11 17,-4 20,-3 31,-7 18,-5 9,-5 3,-9-6,-4-13,-1-10,-4-10,4-7,-1-10</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6235">5043 505,'-9'0,"-13"0,-16 17,-34 23,-24 22,-18 13,-45 37,-24 12,10-11,30-19,39-24,42-21,31-20</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7026">5398 1009,'0'22,"0"24,0 12,-6 6,0 0,1-11</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8493">5425 0,'3'1,"0"-1,1 1,0 0,-1-1,0 1,0 1,0-1,0 0,0 1,0-1,0 0,1 1,-2 0,1 0,-1 1,1-1,-1 1,0-1,0 1,0-1,0 0,-1 1,1 0,-1 0,0 0,1 0,-2 0,1 0,0 0,0 5,4 12,-2 1,0 0,-2 29,-1-34,1 21,1 1,-8 78,5-105,-1-1,0 1,-2-1,1 1,-1-2,0 2,-1-2,0 1,-1-1,-1 0,1 0,-9 9,0-3,-34 31,46-44,1 0,0-1,-1 1,0-1,0 1,0-1,0 1,0-1,0 0,0 0,0-1,0 1,0-1,0 1,0-1,-1 0,1 0,-3 0,3-1,1-1,0 1,0 0,0 0,0-1,0 1,1-1,-1 0,0 2,1-2,-1 0,0 0,0 0,1 0,0 0,0 0,0 0,0-1,0 2,1-1,-1-1,1 1,-1 0,1-1,0-4,-1-5,0 0,1-1,2-15,-1 26,0-1,-1 1,1 0,0-1,0 1,0 0,1 0,-1 0,2 1,-2-1,1 0,-1 0,1 0,0 0,0 1,0-1,0 1,0 0,0-1,0 1,1 0,2 0,60-17,-53 16,40-7,3 1,-2 3,1 2,88 6,-131-2,1-1,-2 2,1 1,19 6,-2 2</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6125,16 +6125,16 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1615 185,'4'0,"11"0,21 0,17 0,5 0,6 0,5 0,27 0,7 0,-6 0,-2 0,-11 0,-12 0,-9 5,-15 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">319 476,'4'5,"2"42,-1 48,0 31,-2 26,-1 5,-1-11,0-30</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2">1 979,'0'-1,"0"0,1 1,-1-1,0 0,1 0,-1 0,1 0,0 0,-1 0,1 1,0-1,-1 0,1 1,0-1,0 0,-1 1,1-1,0 1,0-1,0 1,0 0,0-1,0 1,0 0,2-1,32-6,-27 6,126-15,1 6,151 8,-185 2,-80 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3">1271 238,'24'0,"0"-1,1 1,0 2,-1 0,1 1,43 12,-59-12,269 99,-233-83,-1 3,-1 1,79 58,-105-69,0-1,34 16,-1 0,-48-26,-1-1,0 0,0 1,0-1,0 1,0-1,-1 1,1 0,0 0,0-1,0 1,0 0,-1 0,1 0,0 0,-1-1,1 1,-1 0,1 0,-1 0,1 0,-1 1,0-1,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 1,0-1,-1 0,0 2,-2 1,0 1,0-1,-1 0,1 0,-1 0,0 0,-6 4,-23 18,-1-1,-60 33,-333 148,118-61,266-121,42-24,1 0,0 0,-1 0,1 0,0 0,0 1,-1-1,1 0,0 0,-1 0,1 0,0 0,0 1,-1-1,1 0,0 0,0 0,0 1,-1-1,1 0,0 0,0 1,0-1,0 0,0 0,-1 1,1-1,0 0,0 1,0-1,0 0,0 1,0-1,0 0,0 0,0 1,0-1,0 0,0 1,0-1,0 0,1 1,15 2,35-5,-44 1,14-1,152-7,-146 10,0 0,-1 2,1 1,39 11,-63-14,67 20,108 47,-79-25,-56-28</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4">2859 794,'-35'0,"1"1,-1 2,-45 9,67-9,0 1,0 0,1 1,-1 1,1 0,0 0,0 1,1 1,0 0,1 0,-15 16,-9 10,2 2,1 1,3 1,0 1,-35 71,60-103,0 1,0-1,0 1,1 0,1 0,-1 0,1 0,1 0,-1 0,2 0,-1 0,1 0,0 0,0 0,5 14,-4-17,0-1,1 1,0 0,0-1,0 0,0 0,0 0,1 0,0 0,0 0,0-1,0 0,0 0,1 0,-1-1,1 1,0-1,0 0,0 0,0-1,0 1,0-1,0 0,10 0,51 1,99-10,-146 7,-9-1,0 0,0 0,0-1,0-1,0 0,0 0,-1-1,0 0,0 0,-1-1,1 0,-1-1,0 0,-1 0,0-1,9-11,10-15,-2-2,31-57,-55 92,11-18,0-1,-1 0,-2-1,0 0,-1 0,-1-1,-1 0,-1 1,2-43,-5 46,-3-54,1 69,1 0,-1 0,1 0,-1 0,0 0,0 0,0 1,-1-1,1 0,-1 0,1 1,-1-1,0 1,0-1,0 1,0 0,0 0,-1 0,-3-2,5 3,0 1,-1-1,1 1,-1 0,1 0,0-1,-1 1,1 0,-1 0,1 0,-1 1,1-1,0 0,-1 0,1 1,0-1,-1 1,1-1,0 1,-1 0,1-1,0 1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 1,0-1,1 0,-1 0,0 3,-22 51,22-53,-25 88,-27 187,49-251,0-3,1 1,2 0,0-1,2 25,-1-43,1-1,-1 1,1-1,0 1,0-1,0 0,1 0,0 1,-1-1,2 0,-1 0,0-1,1 1,-1 0,1-1,0 0,1 1,-1-1,0 0,1-1,-1 1,1-1,0 1,0-1,0 0,0-1,6 3,14 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5">3176 1243,'0'-3,"1"-1,0 0,0 0,0 0,1 1,-1-1,1 1,0-1,0 1,0 0,1-1,-1 1,1 0,-1 1,1-1,0 0,5-2,-7 3,1 1,0-1,0 1,0 0,0 0,0-1,0 1,0 1,0-1,0 0,0 0,1 1,-1 0,0-1,0 1,1 0,-1 0,0 0,0 0,1 0,-1 1,0-1,0 1,1-1,-1 1,0 0,0 0,0 0,0 0,0 0,2 3,1 2,0 0,0 0,0 1,-1 0,0 0,-1 0,0 0,0 0,3 13,14 76,-17-81,4 31,-1 0,-3 1,-4 84,0-124,0 0,-1-1,-1 1,1-1,-1 1,0-1,0 0,-1 0,1 0,-1-1,-1 0,1 1,-1-1,0-1,0 1,0-1,-1 0,0 0,0 0,-11 5,-14 5,0-1,-64 18,74-25,14-4,-7 2,0 0,0-1,0 0,0-1,-16 0,28-2,0 0,0 0,0 0,0 0,0-1,0 1,0-1,0 0,0 1,1-1,-1 0,0 0,0 0,1 0,-1 0,1-1,-1 1,-1-2,2 0,0 1,0 0,0-1,0 1,0 0,1-1,-1 1,1-1,0 1,0-1,-1 1,2-1,-1 0,0 1,1-1,-1 1,1 0,1-4,0-1,0 0,1 1,0-1,0 1,1 0,0 0,0 0,0 1,0-1,1 1,0 0,0 0,1 1,-1-1,1 1,0 1,0-1,1 1,-1 0,0 0,1 1,0 0,0 0,0 0,-1 1,1 0,11 0,-2 0,1 1,0 1,-1 0,1 1,-1 0,0 2,0 0,0 1,0 0,25 13,1 6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6">4129 582,'4'0,"11"-4,21-6,21-7,16 1,-5 7,-10 19,-5 20,-3 33,-6 19,-5 9,-5 3,-9-6,-3-13,-2-11,-4-11,5-7,-2-10</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7">4896 529,'-9'0,"-12"0,-16 18,-33 24,-23 23,-18 14,-43 38,-24 13,10-11,29-21,38-24,41-23,30-21</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8">5240 1058,'0'23,"0"25,0 13,-5 6,-1 0,1-11</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9">5267 0,'3'1,"0"-1,0 1,1 0,-1-1,0 1,0 1,0-1,0 0,0 1,0 0,0-1,0 1,-1 0,1 0,-1 1,1-1,-1 1,0-1,0 1,0 0,0-1,-1 1,1 0,-1 0,0 0,1 0,-2 1,1-1,0 0,0 5,3 13,-1 1,0 0,-2 31,-1-37,1 23,1 1,-8 82,5-111,-1 0,0 0,-1 0,0 0,-1-1,0 1,-1-1,0 0,-1 0,0-1,0 0,-9 10,1-3,-34 32,45-46,1 0,0 0,-1 0,0-1,1 1,-1-1,0 1,0-1,0 0,0 0,0-1,0 1,0-1,0 1,0-1,0 0,0 0,-3 0,3-1,1-1,0 1,0 0,0 0,0-1,0 1,1-1,-1 0,0 1,1-1,-1 0,1 0,-1 0,1 0,0 0,0 0,0 0,0-1,0 1,1 0,-1-1,1 1,-1 0,1-1,0-4,-1-6,0 0,1 0,2-17,-1 28,0-1,-1 1,1 0,0-1,0 1,0 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,0 0,0 1,0-1,0 1,0 0,0-1,0 1,1 0,2-1,58-16,-52 16,40-8,2 2,-1 2,0 3,86 6,-127-2,0 0,-1 1,1 1,18 6,-2 3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1664 176,'4'0,"11"0,22 0,18 0,5 0,5 0,7 0,26 0,8 0,-6 0,-2 0,-11 0,-13 0,-9 5,-16 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">329 454,'4'5,"2"40,-1 45,0 30,-2 25,-1 5,-1-11,0-28</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2">1 934,'0'-1,"0"0,1 1,-1-1,0 0,1 0,-1 0,1 0,0 0,-1 0,1 1,0-1,-1 0,1 1,0-1,0 0,-1 1,1-1,0 1,0 0,0 0,0 0,0-1,0 1,1 0,1-1,33-6,-28 6,130-14,1 5,156 8,-191 2,-83 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3">1309 227,'25'0,"0"-1,0 1,1 2,-1 0,1 1,44 11,-61-11,277 94,-239-79,-2 3,-1 1,82 56,-109-67,1-1,34 16,0 0,-50-25,-1-1,0 0,0 1,0-1,0 1,0-1,-1 1,1 0,0 0,0-1,0 1,0 0,-1 0,1 0,0-1,-1 0,1 1,-1 0,1 0,-1 0,2 0,-2 1,0-1,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 1,0-1,-1 0,-1 1,-1 2,0 1,0-1,-1 0,1-1,-1 1,0 0,-7 4,-23 16,-1 0,-61 32,-344 140,121-58,275-115,43-23,1 0,0 0,-1 0,1 0,0 0,0 1,-1-1,1 0,0 0,-1 0,1 0,0 0,0 1,-1-1,1 0,0 0,0 0,0 1,-1-1,1 0,0 0,0 1,0-1,0 0,0 0,-1 1,1-1,0 0,0 1,0-1,0 0,0 1,0-1,0 0,0 0,0 1,0-1,0 0,0 1,0-1,0 0,1 1,15 2,37-5,-46 1,15-1,156-7,-150 10,0 0,-2 2,2 1,40 10,-65-13,69 19,112 45,-82-24,-58-27</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4">2945 757,'-36'0,"1"1,-1 2,-47 9,70-9,0 0,-1 1,2 1,-2 1,2-1,0 1,-1 1,2 0,0 1,0 0,-14 15,-10 9,2 2,1 2,3 0,0 1,-36 68,62-98,0 0,0 0,0 1,1-1,1 1,-1-1,1 1,1 0,-1-1,2 1,-1 0,1-1,0 1,0 0,5 13,-4-17,0 0,1 1,0 0,0-2,0 1,0 0,1 0,0 0,0 0,0-1,0 0,0 0,0 0,1 0,0-1,0 1,0-2,0 1,0 0,0-1,0 1,1-1,-1 0,10 0,53 1,102-10,-150 7,-10-1,0 1,1-1,-1-1,0-1,1 0,-1 0,-1 0,0-1,1 0,-2-1,1 1,-1-2,1 0,-2 1,0-2,10-10,9-15,-1-1,32-55,-57 88,11-17,0-1,0 0,-3-1,0 0,-1 0,0-1,-2 0,-1 1,2-41,-5 44,-3-52,1 66,1 0,-1 0,1 1,-1-1,0 0,0 0,0 1,-1-1,1 0,-1 1,1 0,-1-1,-1 1,1-1,0 1,0 0,0 0,-1 0,-3-1,5 2,0 1,-1-1,1 1,-1 0,1 0,0-1,-1 1,1 0,-1 0,1 0,-2 1,2-1,0 0,-1 0,1 1,0-1,-1 1,1-1,0 1,-1-1,1 0,0 1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 1,0-1,1 0,-1 0,0 3,-23 48,23-50,-26 84,-27 178,49-239,1-3,1 1,2 0,0-1,2 23,-1-40,1-1,-1 1,1-2,0 2,0-1,0 0,1 0,0 0,0 0,1 0,-1 0,0-1,1 1,-1-1,1 0,0 0,1 1,-1-1,0 0,1-1,0 0,0 0,0 1,0-1,0 0,0-1,6 3,15 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5">3271 1186,'0'-3,"1"-1,1 0,-1 0,0 1,1 0,-1-1,1 1,0-1,0 1,0 0,1 0,-1 0,1 0,-1 1,1-1,0 0,6-1,-8 2,1 1,0-1,0 1,0 0,0 0,0-1,0 1,0 1,0-1,0 0,0 0,1 1,-1 0,1-1,-1 1,1 0,-1 0,0 0,0 0,1 0,-1 1,0-1,0 1,1-1,-1 1,0 0,0 0,0 0,1 0,-1 0,2 3,1 1,0 1,0 0,0 1,-1-1,1 1,-2 0,0-1,0 1,3 12,15 73,-18-78,4 30,-1 0,-3 0,-4 81,0-118,0 0,-1-2,-1 2,1-1,-1 1,0-2,0 1,-2 0,2-1,-1 0,-1 0,1 1,-1-2,0 0,0 1,-1-1,0 0,0 0,0-1,-12 6,-14 4,0 0,-65 16,75-23,15-4,-8 2,1 0,0-2,-1 1,1-1,-17 0,29-2,0 0,0 0,0 0,-1 0,1-1,0 1,0-1,0 0,0 1,1-1,-1 0,0 0,0 0,1 0,-1 0,1 0,-1 0,-1-2,2 0,0 1,0 0,0-1,0 1,0 0,1 0,-2 0,2-1,0 1,0-1,-1 1,2-1,-1 0,0 1,2 0,-2 0,1 0,1-4,0-1,0 1,1 0,0-1,0 2,1-1,0 0,0 0,0 2,1-2,0 1,0 0,0 1,1 0,-1-1,2 1,-1 1,0 0,1 0,-1 0,0 0,2 1,-1 0,0 0,0 0,0 1,0 0,11 0,-1 0,0 1,1 1,-2 0,2 1,-2 0,1 2,-1 0,1 1,-1-1,26 14,2 4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6">4253 555,'4'0,"12"-4,21-5,21-7,18 0,-6 8,-11 17,-4 20,-3 31,-7 18,-5 9,-5 3,-9-6,-4-13,-1-10,-4-10,4-7,-1-10</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7">5043 505,'-9'0,"-13"0,-16 17,-34 23,-24 22,-18 13,-45 37,-24 12,10-11,30-19,39-24,42-21,31-20</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8">5398 1009,'0'22,"0"24,0 12,-6 6,0 0,1-11</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9">5425 0,'3'1,"0"-1,1 1,0 0,-1-1,0 1,0 1,0-1,0 0,0 1,0-1,0 0,1 1,-2 0,1 0,-1 1,1-1,-1 1,0-1,0 1,0-1,0 0,-1 1,1 0,-1 0,0 0,1 0,-2 0,1 0,0 0,0 5,4 12,-2 1,0 0,-2 29,-1-34,1 21,1 1,-8 78,5-105,-1-1,0 1,-2-1,1 1,-1-2,0 2,-1-2,0 1,-1-1,-1 0,1 0,-9 9,0-3,-34 31,46-44,1 0,0-1,-1 1,0-1,0 1,0-1,0 1,0-1,0 0,0 0,0-1,0 1,0-1,0 1,0-1,-1 0,1 0,-3 0,3-1,1-1,0 1,0 0,0 0,0-1,0 1,1-1,-1 0,0 2,1-2,-1 0,0 0,0 0,1 0,0 0,0 0,0 0,0-1,0 2,1-1,-1-1,1 1,-1 0,1-1,0-4,-1-5,0 0,1-1,2-15,-1 26,0-1,-1 1,1 0,0-1,0 1,0 0,1 0,-1 0,2 1,-2-1,1 0,-1 0,1 0,0 0,0 1,0-1,0 1,0 0,0-1,0 1,1 0,2 0,60-17,-53 16,40-7,3 1,-2 3,1 2,88 6,-131-2,1-1,-2 2,1 1,19 6,-2 2</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6275,7 +6275,7 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 266,'0'-1,"0"-1,1 1,-1-1,1 1,0 0,-1-1,1 1,0-1,0 1,0 0,0 0,0 0,0-1,0 1,1 0,-1 0,0 1,3-3,29-14,-28 15,22-10,1 2,0 1,1 2,-1 0,55-4,149 4,-221 7,53 0,457 17,72-4,-365-16,172 17,31 0,-262-1,-12 0,657-24,-729 2,84-20,12-2,152-16,162-18,810 18,-427 49,-466-4,-350 2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 253,'0'-1,"0"-1,1 1,-1-1,1 1,0 0,-1 0,1 0,0-1,0 1,0 0,0 0,0 0,0-1,1 1,0 0,-1 0,0 1,3-3,30-13,-28 14,22-9,1 1,1 2,0 1,-1 0,58-3,156 3,-231 7,55 0,478 16,76-3,-382-16,180 16,32 1,-274-2,-12 0,687-22,-763 1,88-18,13-3,158-14,171-18,847 17,-446 47,-489-4,-366 2</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6384,10 +6384,10 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 637,'6'-3,"1"-1,0 1,-1 0,1 0,1 1,-1 0,0 0,1 1,-1 0,1 0,-1 1,14 1,-5-2,-14 1,41-2,55 3,-96-1,-1 1,1-1,-1 0,1 0,-1 1,0-1,1 1,-1-1,1 1,-1-1,0 1,1 0,-1 0,0 0,0-1,0 1,0 1,0-1,0 0,0 0,0 0,0 0,0 1,0-1,-1 0,1 1,-1-1,1 0,-1 1,1-1,-1 1,0-1,0 1,1-1,-1 1,0-1,-1 1,1-1,0 1,-1 1,-1 9,0-1,-2 1,1-1,-8 15,2-3,0 15,1 1,2 0,1 0,2 73,3-102,-1 41</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1585.99">1403 505,'67'-5,"-52"3,0 0,0 1,1 1,-1 0,27 4,-38-3,0 1,0-1,0 1,0-1,0 1,0 1,0-1,-1 0,1 1,-1 0,0-1,0 2,0-1,0 0,0 0,-1 1,1 0,-1-1,0 1,0 0,0 0,-1 0,1 0,1 9,3 24,-1 1,-2 0,-2 0,-7 72,2-27,3-45</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3154.99">2356 2,'25'-1,"41"0,-63 2,-1-1,1 0,-1 0,1 1,-1 0,1-1,-1 1,0 0,1 0,-1 0,0 0,0 1,0-1,0 1,0-1,0 1,0 0,0-1,-1 1,3 4,0 4,0 1,-1-1,0 1,-1 0,-1 0,1 0,-2 0,1 0,-2 0,-1 12,-22 120,14-97,10-46,-6 33,-2 0,0-1,-16 36,18-51,1 0,1 0,1 1,0-1,1 1,1 0,0-1,3 26,-1-19,-1 1,-1-1,-5 32,0-33</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4825.99">3705 320,'4'0,"7"0,5 0,4 0,4 0,-2 5,-5 10,-6 7,-4 4,-4 3,-2 0,-1 5,-1 1,0-2,0-1,0-1,1 2,0-4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 621,'6'-3,"2"-1,-1 1,-1 0,2 0,0 2,-1-1,1 0,0 1,-1 0,2 0,-2 1,15 1,-5-2,-15 1,43-2,58 3,-101-1,-1 1,1-1,-1 0,1 0,-1 1,0-1,1 1,-1-1,2 1,-2-1,0 1,1 0,-1 0,0 0,0-1,0 0,0 2,0-1,0 0,0 0,0 0,0 0,0 1,0-1,-1 0,1 1,-1-1,1 0,-1 1,1-1,-1 1,0-1,0 1,2-1,-2 1,0-1,-2 1,2-1,0 1,-1 1,-1 8,0 0,-2 1,1-2,-9 16,3-4,-1 15,2 1,2 0,1 0,1 72,4-101,-1 41</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1585.99">1471 492,'70'-5,"-54"4,0-1,-1 1,2 1,-1 0,28 4,-40-4,0 2,0-1,1 1,-1-1,0 1,0 1,0-1,0 0,0 1,-1 0,0-1,0 2,0-1,0 0,1 0,-2 0,1 1,-1-1,0 1,0 0,0 0,-1 0,1 0,2 8,2 25,-1 0,-2 0,-2 0,-7 70,2-26,3-44</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3154.99">2470 2,'26'-1,"43"0,-65 2,-2-1,1 0,-1 0,1 1,-1 0,1-1,-1 1,1 0,0 0,-1 0,0 0,0 1,0-1,0 1,0-1,0 1,0 0,1-1,-2 0,3 5,0 4,0 1,-1-1,0 0,0 1,-2 0,1-1,-2 1,1 0,-2 0,-1 11,-24 117,16-94,10-45,-6 32,-3 1,1-2,-17 35,18-49,2-1,1 1,1 0,0 0,1 1,1-1,0 0,3 25,-1-19,-1 1,-1 0,-6 30,1-31</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4825.99">3884 312,'5'0,"6"0,6 0,4 0,4 0,-2 5,-5 9,-7 8,-3 3,-5 4,-2-1,-1 5,-1 1,0-2,0-1,0 0,1 1,0-4</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6414,7 +6414,7 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1784,'29'26,"2"-5,2 0,-1-3,2 0,1-2,0-2,1-1,0-2,0-1,2-2,-1-2,64 3,608-15,-324-21,-217 5,130-9,-146 27,177-27,-41-13,280-51,-486 79,107-26,-166 35,0-1,0-1,0-1,-1-2,37-24,3-5,3 3,72-32,-66 36,113-74,4-42,-84 64,-41 39,31-27,-40 25,148-123,-191 162,0 0,-1 0,0-1,-1-1,0 1,0-2,8-16,24-32,6 5,4 3,63-53,-63 61,-2-2,86-105,-84 87,-35 50</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1747,'30'25,"3"-4,2 0,-2-4,3 1,0-3,1-1,1-1,0-2,-1-2,3-1,-1-2,67 3,637-15,-339-20,-228 4,136-8,-152 26,185-26,-43-14,293-49,-509 78,112-26,-174 34,0-1,1-1,-1-1,-1-1,39-25,3-4,3 3,75-32,-68 36,118-73,4-41,-88 63,-43 38,33-26,-43 24,156-121,-201 160,1-1,-2 0,1-1,-2-1,1 2,-1-3,9-15,25-32,6 5,5 3,65-52,-65 60,-3-2,91-103,-89 86,-36 48</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6441,7 +6441,7 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 2222,'88'5,"142"24,-93-8,-67-11,-27-3,72 3,2045-12,-2108-1,-1-2,0-3,-1-2,70-23,-44 12,-61 17,75-19,139-57,-168 57,102-24,-87 26,14-7,-2-3,-1-4,125-71,-193 95,71-39,147-109,-222 147,0-1,0-1,-1 0,-1-1,0 0,15-26,49-69,-48 72,-2-2,27-51,-14 20,4 2,102-125,-131 175,94-107,-63 75,-1-2,52-82,-36 40,-35 58,-2-2,-1 0,28-69,4-31,-47 114</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 2169,'92'5,"149"23,-97-7,-71-12,-28-2,76 3,2142-12,-2209-1,0-2,-1-3,0-1,72-24,-45 13,-64 16,78-18,146-56,-176 55,107-23,-92 26,16-8,-3-2,-1-4,131-70,-202 94,74-39,155-106,-233 143,-1-1,1 0,-1-1,-2-1,1 1,15-26,52-68,-51 71,-1-2,27-50,-14 20,4 2,107-123,-137 172,98-105,-66 73,-1-2,55-80,-38 40,-37 56,-2-2,-1 0,30-68,4-30,-50 112</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6632,16 +6632,16 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">3228 0,'-2'0,"0"0,1 0,-1 1,0-1,1 0,-1 1,0-1,1 1,-1-1,1 1,-1 0,1-1,-1 1,1 0,-1 0,1 0,0 0,0 0,-1 1,0 1,-18 36,19-37,-108 312,4-9,-239 522,128-320,203-478,2 1,1 0,2 0,0 1,3 0,0 0,0 35,-39 387,-1 62,42-470,-2 1,-12 48,-3 31,-68 519,32-272,41-274,7-36,-22 79,14-87</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1439.99">1 2884,'736'-26,"16"-5,6 33,-289 0,167-3,649 3,-531 35,-170-4,965-21,-954-15,405 3,-966 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4228">1191 3731,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4576">2302 3413,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4938">2726 2990,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5304">3202 2540,'0'-4,"4"-6,2-2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5797">4657 1879,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6145.02">5768 1323,'4'-4,"2"-2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6496.03">6694 1006,'4'-4,"2"-2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6874.99">7832 529,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">3358 0,'-2'0,"0"0,1 0,-1 1,0-1,1 0,-1 1,0-1,0 1,0-1,1 1,-1 0,1-1,-1 1,1 0,-1 0,1 0,0 0,0 0,-1 1,0 1,-19 34,20-35,-112 304,3-10,-248 508,134-311,210-465,3 1,0 0,3 1,0 0,2 0,1 0,0 34,-41 376,0 61,42-457,-1 0,-13 48,-2 29,-72 505,34-264,42-267,8-35,-23 78,14-86</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1439.99">1 2803,'766'-25,"16"-5,7 32,-302 0,175-3,675 3,-553 34,-176-4,1003-20,-992-15,422 3,-1006 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4228">1239 3627,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4576">2395 3318,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4938">2836 2906,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5304">3331 2469,'0'-4,"4"-6,2-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5797">4845 1826,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6145.02">6000 1286,'5'-4,"1"-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6496.03">6964 978,'4'-4,"2"-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6874.99">8148 514,'0'0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6668,14 +6668,14 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">2938 0,'3'71,"25"132,-13-109,299 2127,-245-907,-7-374,-19-289,-26-354,11-99,-10-102,-12-51</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="920.96">1 3916,'233'-73,"-78"21,219-53,766-108,-181 173,-722 40,1202-23,748-1,-1996 10,-31 2,-6 14,-76 1,133-12,-181 3,-10 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2125.96">742 926,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2634.96">1033 1720</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3152.96">2355 2778,'4'0,"2"0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3734.98">3784 3202,'4'0,"7"0,5 0,0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4273">5822 2672,'4'0,"6"0,2 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4828.96">7462 1455,'4'0,"2"0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">3082 0,'3'69,"26"129,-13-106,313 2074,-256-884,-8-365,-20-282,-27-346,11-96,-10-99,-13-50</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="920.95">1 3820,'244'-72,"-81"22,229-53,804-105,-190 169,-758 39,1262-22,784-1,-2094 9,-32 2,-7 14,-79 1,140-12,-191 3,-10 2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2125.96">778 903,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2634.96">1083 1678</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3152.96">2470 2710,'4'0,"3"0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3734.98">3969 3123,'4'0,"8"0,4 0,1 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4273">6107 2606,'4'0,"6"0,3 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4828.96">7827 1419,'4'0,"2"0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6702,13 +6702,13 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">2568 0,'-54'212,"8"-39,-130 933,135-786,-45 454,61 6,26-727</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="662.99">1 1879,'1'-2,"1"0,0 0,-1-1,1 1,0 0,1 1,-1-1,0 0,0 1,1-1,-1 1,1-1,-1 1,6-1,43-11,-41 11,113-16,1 6,180 5,-187 6,1144 14,1 99,-364 35,-853-139,291 36,-332-44,1 0,1 0,-1 0,0 1,0-1,0 1,0 0,0 1,0-1,0 1,-1 0,1 0,-1 1,1-1,-1 1,8 6,-2 6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1441">716 2249,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2021.99">1589 1191,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2545.99">2647 1111,'4'0,"11"5,8 1,3 4,-2 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3049">3891 1958,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3599.99">4288 2778,'4'0,"7"5,0 10,9 7,8 18,10 7,20 17,1-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">2670 0,'-56'206,"8"-38,-135 907,140-764,-46 441,63 6,27-707</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="662.99">1 1826,'1'-2,"1"0,0 0,-1-1,1 1,0 0,2 1,-2-1,0 0,0 1,1-1,-1 1,1-1,-1 1,6-1,45-10,-42 10,117-16,1 7,187 4,-195 6,1190 14,1 95,-378 35,-887-135,302 35,-345-43,1 0,2 0,-2 0,0 1,0-1,0 1,1 0,-1 1,0-1,0 1,-1-1,2 1,-2 1,1-1,-1 1,9 6,-3 6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1441">744 2185,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2021.99">1652 1157,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2545.99">2752 1079,'4'0,"12"5,8 1,3 4,-2 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3049">4045 1902,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3599.99">4458 2699,'4'0,"7"5,1 10,9 6,8 18,10 7,22 16,0-1</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6762,8 +6762,8 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">3494 0,'10'191,"0"-35,-7 257,26 394,65-110,25 303,-70-52,-50-3,-13-755,-8-1,-66 264,81-423,-53 240,50-209,3 1,0 90,11 12,-3-119</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1234.99">1 3995,'0'-1,"1"0,-1 0,1 0,-1 0,1 0,0 0,-1 0,1 0,0 0,0 0,0 0,0 1,0-1,0 0,0 1,0-1,0 0,0 1,0 0,1-1,-1 1,0-1,0 1,0 0,1 0,-1 0,1 0,44-5,-39 5,601-6,-317 9,919 0,1694-6,-2240-10,226-1,324 14,-860 28,-113-5,-191-20</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">3646 0,'10'186,"1"-34,-8 250,27 383,68-106,26 294,-72-50,-53-3,-14-735,-8-1,-69 257,85-412,-56 234,53-204,2 2,1 87,11 11,-3-115</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1234.99">1 3889,'0'-1,"1"0,-1 0,1 0,-1 0,1 0,0 0,-1 0,1 0,0 0,0 0,0 0,0 1,0-1,0 0,1 1,-1-1,0 0,0 1,0 0,1-1,-1 1,0-1,0 1,0 0,1 0,-1 0,1 0,46-5,-41 5,628-5,-331 8,958-1,1769-4,-2339-11,237-1,338 14,-898 28,-117-6,-200-19</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6790,7 +6790,7 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 4651,'8'0,"0"-1,0 0,0 0,0-1,0 0,-1-1,1 0,-1 0,1 0,-1-1,0 0,0-1,-1 1,1-1,-1-1,0 1,7-9,8-11,-2-2,0 0,16-31,6-8,58-94,-93 146,0 1,-1-1,-1 0,0 0,-1 0,2-24,-3 20,1 1,1 0,0 0,7-16,9-19,14-61,-23 70,2 1,32-69,-25 72,-1-2,-2 1,-2-2,18-77,-28 88,1 0,1 1,2 0,1 0,1 1,2 0,20-33,89-116,103-169,-209 317,118-204,-105 189,3 1,73-78,-12 30,108-115,-176 177,-1-2,-2 0,-1-2,-2 0,21-51,-22 47,2 1,2 0,0 2,3 1,1 0,1 2,45-40,-64 64,1 2,0 0,0 0,0 0,1 1,-1 0,17-4,77-19,-23 8,23-15,78-22,-106 36,97-22,-151 39,1 1,0 1,0 1,0 2,42 4,-51-1,1 1,-1 0,0 1,-1 1,1 0,-1 0,-1 1,0 1,0 0,13 13,31 24,-29-25,0 2,-2 0,-1 2,28 37,-16-19,-11-9,-1 1,-1 1,28 66,18 30,101 121,-75-111,21 27,-97-143,0 2,13 30,-14-26,24 37,171 213,-160-211,3-3,119 114,-94-103,88 111,45 46,-183-206,2-2,1-2,2-1,0-1,56 27,-76-45,0 0,1-1,0-1,0 0,0-1,25 1,97-5,-77-1,238 2,159-5,-418 2,0-2,-1-1,0-2,0-2,-1-1,64-29,-48 14,-2-2,-1-3,88-70,-56 30,94-103,51-88,-96 90,167-286,-219 310,97-253,-153 344,54-142,-21 48,131-244,-113 253,-52 94,2 1,1 2,3 0,55-64,-29 44,-3-2,44-76,54-70,-114 169</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 4541,'8'0,"1"-1,-1 0,1 0,-1-1,0 0,0-1,0 0,-1 0,2 0,-2 0,1-1,-1-1,-1 1,2-1,-2-1,0 1,8-8,8-12,-2-1,0-1,17-29,6-9,60-91,-96 142,-1 2,-1-2,0 0,-1 1,-1-1,2-23,-3 19,1 2,2-1,-1 1,7-17,10-17,15-61,-24 69,1 1,34-67,-26 70,-1-2,-2 1,-2-2,19-75,-30 85,1 1,2 1,1 0,1-1,2 2,2 0,20-33,94-113,109-165,-221 310,125-199,-110 184,2 1,77-76,-12 29,113-112,-185 172,-1-1,-1 0,-2-2,-2 0,22-50,-24 46,3 0,3 1,-1 2,3 1,1 0,2 1,46-38,-67 62,2 2,-1 1,1-1,-1 0,2 1,-2 0,19-4,80-18,-24 7,24-14,82-21,-111 34,101-21,-158 38,1 1,0 1,0 1,1 2,43 4,-54-1,2 1,-1 0,-1 1,0 1,1-1,-2 1,0 1,-1 1,1 0,13 12,33 24,-31-24,0 1,-1 1,-2 1,29 36,-16-18,-12-8,-1 0,-1 1,30 65,18 28,107 119,-80-108,23 26,-102-140,0 3,14 28,-16-24,26 35,180 208,-168-205,2-4,126 112,-99-101,92 108,48 46,-193-202,3-2,1-1,1-2,1 0,59 25,-81-43,1 0,1-1,0-1,0 0,-1-1,27 1,102-5,-81-1,250 2,167-5,-439 2,0-2,-1-1,0-2,0-1,-1-2,67-28,-50 13,-3-1,0-3,92-69,-59 30,99-101,53-86,-100 88,174-279,-229 303,102-248,-161 336,57-138,-22 47,138-239,-120 247,-54 93,3 0,0 2,3 0,59-63,-32 44,-2-2,46-75,56-68,-119 165</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6900,8 +6900,8 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 2714,'0'-1157,"1"1140,0 0,2 0,0 0,1 1,0 0,1 0,1 0,1 0,0 1,19-29,-13 25,2 0,-1 0,2 2,1 0,0 1,1 0,23-15,-8 12,1 2,1 1,61-19,-6 2,116-41,-170 64,0 1,1 2,70-4,79 9,165-10,-299 10,0 3,1 2,-1 2,0 2,-1 2,0 3,0 2,-2 2,70 33,-6 6,-4 6,181 131,-140-93,-92-64,-1 3,67 60,-82-60,59 54,149 174,-245-259,137 182,-115-148,-1 1,35 82,123 320,-80-202,-92-218</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1254">3017 809,'35'-65,"3"2,54-70,102-104,-99 125,-61 71,-7 6,63-61,-88 94,1-1,0 1,-1 0,1 0,0 0,0 0,0 0,0 0,0 1,0 0,1-1,-1 1,0 0,1 1,-1-1,1 1,-1-1,1 1,5 1,-6 0,-1 0,1 1,-1-1,1 1,-1 0,1-1,-1 1,0 1,0-1,0 0,0 0,-1 1,1-1,-1 1,1-1,-1 1,0 0,0-1,0 1,0 0,0 0,0 5,8 51,-3-1,-2 1,-3 0,-6 61,2-20,-9 608,12-696,1 0,0 0,0 0,7 22,-3-16</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 2643,'0'-1126,"1"1109,0 0,2 1,0-1,2 2,-1-1,1 1,1-1,2 0,-1 2,20-29,-13 24,2 1,-2-1,3 3,1-1,0 2,0-1,25-14,-8 11,1 3,0 0,65-18,-7 2,122-40,-179 62,1 1,1 3,73-5,83 9,172-10,-312 10,-1 3,2 2,-2 2,1 2,-2 2,1 2,-1 3,-2 2,74 31,-7 7,-3 5,188 128,-146-90,-96-63,-1 3,70 58,-86-58,62 53,155 169,-255-252,142 177,-119-144,-2 1,37 79,128 313,-83-197,-96-213</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1254">3160 788,'37'-63,"2"1,58-67,106-102,-104 122,-63 69,-8 6,67-60,-93 92,1-1,0 1,-1 1,1-1,0 0,1 0,-1 0,0 0,0 1,0 0,1-1,-1 1,1 0,0 1,-1-1,1 1,-1-1,1 1,6 1,-7 0,-1 0,1 1,-1-1,1 1,0 0,0-1,-1 1,0 1,0-1,0-1,0 1,-1 1,1-1,-1 1,1-1,0 1,-1 0,0-1,0 1,0 0,0 0,0 5,8 49,-2-1,-3 2,-3-1,-6 60,1-19,-8 591,12-677,1 0,0-1,0 1,7 21,-2-15</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6928,7 +6928,7 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 516,'11'2,"0"1,1 0,-1 0,-1 1,1 1,0 0,-1 0,0 1,0 0,10 9,21 11,36 12,124 45,-73-34,-51-16,0 3,-3 3,99 69,-92-50,587 399,-624-429,219 143,-213-135,-3 3,-1 1,44 52,5 12,122 106,-155-158,1-3,3-4,110 59,406 219,-246-131,-18 3,-155-92,265 143,-140-86,-61-28,129 79,-351-208,-1-1,1 1,-1-1,1 0,0 0,0 0,0-1,0 0,0 0,7 0,-1-1,0 0,0-2,0 1,14-5,291-78,-82 18,1934-528,-2102 576,42-13,154-65,-241 86,-1-2,-1 0,0-2,20-16,34-25,37-8,209-87,-147 75,-80 32,442-208,-17-35,-391 199,226-207,-190 152,-28 27,339-282,92-78,-430 353,109-104,-128 120,-26 27,-60 48,-19 19,0 1,1 0,0 1,0 0,20-11,-32 20,0 1,0 0,0 0,1 0,-1-1,0 1,0 0,1 0,-1 0,0 0,0-1,1 1,-1 0,0 0,1 0,-1 0,0 0,0 0,1 0,-1 0,0 0,1 0,-1 0,0 0,1 0,-1 0,0 0,0 0,1 0,-1 1,0-1,0 0,1 0,-1 0,0 0,0 0,1 1,-1-1,0 0,0 0,1 1,-1-1,0 0,0 0,0 1,0-1,0 0,1 0,-1 1,0-1,0 0,0 1,-2 17,1-17,-8 30</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 502,'11'2,"1"1,0 0,0 0,-2 1,2 1,-1-1,0 1,-1 1,0 0,11 9,22 10,37 12,129 44,-75-34,-54-15,0 3,-3 3,103 68,-95-50,610 389,-649-418,228 139,-222-131,-3 3,-1 1,46 51,4 11,128 103,-161-153,1-3,2-5,116 59,422 212,-257-127,-17 2,-163-88,277 138,-146-83,-64-28,135 78,-366-204,-1 0,2 1,-2-1,1 0,0 0,0 0,1-1,-1 0,0 0,7 0,0-1,-1 0,1-2,-1 1,15-5,303-75,-85 16,2014-513,-2190 561,45-13,160-64,-252 84,0-1,-1-1,0-2,20-15,36-24,39-9,217-84,-153 74,-83 30,460-203,-17-33,-408 193,235-201,-197 148,-30 26,354-274,95-76,-447 343,113-101,-133 117,-27 26,-63 47,-20 18,1 2,0-1,1 1,-1 0,21-10,-33 19,0 1,0 0,0 0,2 0,-2-1,0 1,0 0,1 0,-1 0,0 0,0-1,1 1,-1 0,0 0,1 0,-1 0,0 0,0 0,1 0,-1 0,0 0,1 0,-1 0,0 0,1 0,-1 0,0 0,0 0,1 0,-1 1,0-1,0 0,1 0,-1 0,0 0,0 0,1 1,-1-1,0 0,0 0,1 1,-1-1,0 0,0 0,0 1,0-1,0 0,1 0,-1 1,0-1,0 0,0 1,-2 16,1-16,-9 29</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6955,7 +6955,7 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">6 1939,'-3'-79,"1"48,1 1,2-1,0 1,2 0,13-55,13 2,3 2,3 1,5 2,48-74,216-279,-302 429,54-76,60-74,-99 134,0 1,1 0,1 1,0 1,40-23,102-57,27-15,-145 89,2 3,0 1,1 2,73-13,191-16,-22 27,-231 18,0 2,-1 3,59 13,-73-7,0 1,49 25,3 1,-43-21,-2 3,0 1,-1 3,-2 2,74 55,-59-32,259 219,-226-183,103 123,-159-158,-2 1,40 79,-43-71,8 14,-4 3,36 104,-68-167,-2 0,1 0,-2 1,1 16,-2-9</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">6 1898,'-3'-77,"1"46,1 2,2-1,0 0,2 1,14-54,13 1,4 3,2 1,6 2,50-73,226-273,-316 420,57-74,62-73,-103 131,0 1,0 1,2 0,0 1,42-22,106-56,29-14,-152 86,2 3,0 2,1 1,76-12,200-16,-23 26,-241 18,0 2,-2 3,62 12,-76-6,0 1,51 24,4 1,-46-20,-2 2,1 2,-2 2,-2 3,77 53,-61-31,271 214,-237-178,108 119,-166-154,-3 1,43 77,-46-69,9 13,-4 4,37 101,-71-163,-2-1,2 1,-3 1,1 15,-2-8</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6982,7 +6982,7 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">61 2437,'-5'-10,"2"-1,0 0,0 1,1-2,0 1,0-12,-3-16,-13-89,7 0,5-1,13-159,-6 275,1-1,0 1,0 0,2-1,-1 1,2 1,0-1,0 1,8-13,1 5,0 0,1 1,1 0,28-24,568-547,-510 475,-61 66,-24 32,2 1,0 1,1 0,0 2,1 0,30-13,-17 8,257-132,-211 114,146-45,-147 58,66-19,1 5,159-17,-137 34,179-14,1011 24,-790 14,-301-7,276 6,-300 17,-152-11,22 5,0 4,-1 6,130 45,-99-18,265 138,-306-135,150 85,-196-104,-2 2,69 62,262 246,-303-273,257 235,-317-283,0 0,-3 2,0 0,-1 1,-1 1,-2 1,-1 0,-2 1,0 0,8 39,-14-32,-1 1,-3-1,-1 1,-5 58,0-2,4-65</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">64 2368,'-6'-10,"3"0,0-1,0 1,1-1,0 0,0-11,-4-16,-12-87,6 1,6-1,13-155,-6 267,1-1,1 2,-1-1,2 0,-1 0,2 1,0 0,1 0,7-12,2 4,-1 1,2 0,1 1,28-24,593-531,-531 461,-65 64,-24 32,2 0,0 2,1-1,0 3,0-1,33-12,-19 7,268-128,-219 111,151-43,-152 55,68-17,1 4,166-17,-143 34,187-14,1054 23,-824 14,-314-7,288 6,-313 16,-158-10,23 5,0 3,-1 6,135 45,-103-19,276 135,-318-132,155 83,-203-101,-3 2,72 60,273 240,-315-266,267 228,-330-275,0 1,-3 1,0 0,-1 1,-2 2,-1 0,-2 0,-1 1,0 0,7 38,-13-31,-2 1,-3-1,-1 1,-5 56,0-1,4-64</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7036,16 +7036,16 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">4532 0,'0'4783,"0"-3388,-2-1354,-2-1,-2 0,-19 70,22-96,-4 15</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="997.99">8 4021,'-1'0,"0"-1,1 0,-1 0,0 0,1 1,-1-1,1 0,-1 0,1 0,0 0,-1 0,1 0,0 0,0 0,-1 0,1 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,1 0,-1 0,0 0,1 0,-1 0,1 0,-1 0,1 0,0 0,-1 1,1-1,0 0,-1 0,1 1,0-1,0 1,0-1,0 0,0 1,1-1,49-25,-47 24,98-36,1 4,3 4,0 5,172-17,450 6,-420 28,660-16,0 58,90 80,300 21,-189-102,6-39,-185 0,-641-9,-341 14,52-1,-46 5</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4936.99">1252 5582,'2'0,"0"0,1-1,-1 0,1 0,-1 1,0-1,0-1,0 1,1 0,-1 0,0-1,-1 1,1-1,0 0,0 0,-1 1,1-1,-1 0,2-3,28-49,-22 36,18-36,-3-1,32-106,11-123,-54 192,-3 0,-5-1,-8-116,5-110,2 272,2 0,2 0,2 1,27-79,-2 45,3 0,3 3,4 2,3 1,3 3,91-98,-116 140,1 2,2 1,50-36,-63 52,1 0,1 1,0 0,0 2,0 0,1 1,0 1,39-5,-11 4,2 2,-1 2,0 3,84 11,-109-6,0 1,-1 1,0 1,0 1,-1 1,-1 1,34 25,124 120,-139-121,-3 0,-2 1,-2 2,46 73,64 138,-141-249,23 51,19 56,-6-14,137 269,-112-254,63 103,-99-174,1 0,2-3,43 42,-37-47,1-1,2-2,0-2,2-1,76 33,-63-39,1-2,0-2,1-3,1-2,-1-3,87-1,-108-5,-1-2,1-1,-1-2,0-1,0-1,61-24,-68 21,0-2,-1 0,-1-2,-1-1,0-1,0-1,-2 0,34-37,55-57,-23 25,29-61,-32 38,-65 87,276-348,-162 192,31-43,108-148,-176 244,115-131,-178 226,1 0,1 2,2 2,46-25,-50 32,0 2,2 1,0 1,0 3,45-11,-67 20,0 1,1 0,-1 0,1 2,-1 0,1 0,-1 1,1 1,-1 0,0 1,0 0,0 1,0 1,-1 0,1 1,-1 0,-1 0,13 10,9 12,0 1,-3 2,0 2,-2 0,-1 2,38 65,104 243,-142-282,102 265,-80-220,29 75,102 207,-60-143,-115-233,118 240,-98-207,2-1,3-2,48 56,-31-48,74 89,-104-117,-2 1,0 0,-2 2,19 45,175 433,5-89,-187-374,61 71,-66-86,2 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6576.03">2654 3704,'2'-20,"2"-1,0 1,2 0,0 0,1 1,1 0,1 0,11-18,-12 22,-3 4,1-1,0 0,1 0,0 0,0 1,18-20,-24 31,0-1,0 0,-1 0,1 0,0 1,0-1,0 1,0-1,0 1,0-1,0 1,0-1,0 1,0 0,0 0,1-1,-1 1,0 0,0 0,0 0,0 0,0 0,0 0,0 1,0-1,1 0,-1 1,0-1,1 1,1 1,-1 0,0 0,1 0,-1 0,0 1,0-1,0 1,-1-1,1 1,2 4,2 7,-1 1,0-1,4 21,0 21,-3 0,-1 70,-4-76,1 0,3 0,15 69,-13-94</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7854.99">4559 4603,'0'-3,"1"-1,0 0,0 0,0 0,1 1,-1-1,1 0,0 1,0-1,0 1,1 0,-1 0,1 0,-1 0,1 0,0 1,0-1,1 1,5-4,-2 1,1 0,1 1,-1 0,0 0,1 1,0 0,11-2,-18 5,0 0,1 0,-1 0,0 0,0 0,0 1,1-1,-1 1,0-1,0 1,0 0,0 0,0 0,0 0,0 0,0 0,-1 1,1-1,0 1,-1-1,1 1,-1 0,1-1,-1 1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,-1 0,1 0,-1 1,1 2,2 11,-1-1,-1 1,0 27,-1-38,0 2,1 0,-2 0,1 0,-1 0,0 0,0 0,-1 0,0 0,0-1,0 1,-1-1,0 1,0-1,-1 0,0 0,0-1,0 1,-1-1,0 0,0 0,0 0,-1-1,-10 7,16-10,0-1,-1 0,1 0,-1 0,1 0,-1 0,1 1,0-1,-1 0,1 0,-1 1,1-1,0 0,-1 1,1-1,0 0,-1 1,1-1,0 0,0 1,-1-1,1 1,0-1,0 0,0 1,-1-1,1 1,0-1,0 1,0-1,0 1,0-1,0 1,0-1,0 1,18 7,50 0,-40-6,227 49,-215-44</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9326">7893 2143,'101'-2,"109"4,-187 0,0 0,-1 2,0 1,0 1,0 0,40 19,-59-23,0-1,-1 0,1 1,0 0,-1 0,1-1,-1 1,0 1,0-1,0 0,0 1,0-1,0 1,0-1,-1 1,1 0,-1 0,0 0,0 0,0 0,0 0,-1 0,1 0,-1 0,0 0,1 0,-2 0,1 0,0 0,-1 1,1-1,-1 0,-1 4,-1 1,0-1,-1 0,1 0,-1-1,-1 1,1-1,-1 0,0 0,-1 0,1-1,-1 1,-9 5,0-2,10-6,0 0,0 0,0 1,1-1,-1 1,1 0,-5 6,9-9,-1 0,1-1,-1 1,1 0,0 0,-1 0,1 0,0-1,0 1,0 0,0 0,-1 0,1 0,0 0,1 0,-1 0,0 0,0-1,0 1,1 2,0-1,0 0,1 0,-1-1,0 1,1 0,-1-1,1 1,0-1,0 1,-1-1,1 0,3 2,74 37,-60-32,0 0,-1 2,0 0,0 1,-2 1,19 16,-31-23,0 0,-1 0,0 1,0-1,0 1,0 0,-1 0,0 0,0 0,-1 0,0 0,0 1,0-1,-1 0,0 1,0-1,0 0,-2 8,0-4,1 0,-2 0,1 0,-1 0,-1-1,0 0,0 1,-1-1,0-1,-9 14,4-12,1 0,-1-1,-1 0,0 0,0-1,0-1,-1 0,-1 0,1-1,-1-1,-17 5,6-3,-1-2,-1-1,1-1,-1-1,-30-1,33-2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11194.99">9612 529,'-33'2,"1"1,0 2,0 1,0 1,1 2,-38 15,50-18,-1 2,1 0,-28 17,40-20,1 0,0 0,0 0,0 1,0 0,1 0,0 0,0 1,1 0,0 0,0 0,-4 10,-2 16,0 1,3 0,0 1,3-1,0 1,4 63,0-89,0 0,1-1,1 1,0 0,0 0,0-1,1 1,0-1,1 0,0 0,0 0,6 8,-1-5,0-1,0 1,1-2,0 1,1-1,0-1,13 9,5-1,0-2,0 0,2-2,-1-2,61 14,-85-23,0 1,0-1,0 0,0 0,0-1,0 0,0 0,1 0,-1-1,0 1,0-2,0 1,-1-1,1 1,0-2,0 1,-1-1,0 0,1 0,-1 0,0-1,-1 1,1-1,0-1,-1 1,0 0,0-1,5-8,13-17,20-26,47-83,-79 120,-1 0,0-1,-1 0,-2-1,0 1,-1-1,0 0,1-41,-10-136,4 195,0 1,-1-1,1 1,-1-1,0 1,0-1,1 1,-1 0,-1-1,1 1,0 0,-1 0,1 0,-1 0,1 0,-1 0,0 0,0 0,0 1,0-1,0 1,0 0,-3-2,-1 1,-1 0,1 0,-1 0,1 1,-1 0,0 0,-10 0,-8 2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12224">10089 1190,'0'5,"0"6,0 14,0 17,-5 5,-1 0,0-4,1-5,7-9,11-22,8-22,5-13,7-11,-2-2,-2 5,-1 8,-6 10</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12935">11359 423,'-2'11,"1"0,-1 0,-1 0,0 0,0-1,-1 0,-1 1,-5 9,0 0,-142 284,-45 99,193-393,-1 1,2-1,-1 1,1 0,1 0,0 0,-1 17,3-24,1-1,-1 0,1 1,0-1,0 0,0 0,0 0,0 0,1 0,0 0,-1 0,1 0,0-1,0 1,0 0,1-1,-1 0,1 0,-1 1,1-2,0 1,0 0,0 0,0-1,0 0,0 1,0-1,0 0,5 0,33 8,0-1,1-3,0-1,69-3,-87-2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13522.02">11650 238,'-5'98,"-33"182,17-159,-131 580,38-214,52-17,60-451,-1 12</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">4711 0,'0'4664,"0"-3304,-2-1320,-2-1,-3 0,-19 68,23-93,-4 14</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="997.99">8 3921,'-1'0,"0"-1,1 0,-1 0,0 0,1 1,-1-1,1 0,-1 0,1 0,0 0,-1 0,1 0,0 0,0 0,-1 0,1 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,1 0,-1 0,0 0,1 0,-1 0,1 0,-1 0,1 0,0 0,-1 1,1-1,0 0,-1 0,1 1,0-1,0 1,0-1,1 1,-1 0,1-1,51-25,-49 24,102-35,1 4,3 4,0 4,179-16,468 6,-437 28,686-17,1 57,92 78,313 21,-197-100,7-38,-193 1,-667-10,-353 14,53-1,-47 5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4936.99">1301 5443,'3'0,"-1"0,1-1,-1 0,1 0,-1 1,0-1,0-1,0 1,1 0,-1 0,0-1,0 1,0-1,0 0,0 0,-1 1,1-1,-1 0,2-3,29-47,-22 34,18-35,-3 0,33-104,11-120,-55 187,-4 1,-4-2,-10-113,7-107,1 265,2 0,2 1,3 0,27-77,-1 44,2 0,4 3,3 2,4 0,3 4,95-96,-121 137,1 2,2 0,52-34,-65 50,1 1,0 0,1 0,0 2,-1 0,2 1,0 2,40-6,-11 4,2 2,-1 2,0 3,87 11,-113-6,0 1,-1 0,0 2,-1 1,0 1,-1 0,35 25,129 117,-144-117,-4-1,-1 1,-3 2,48 71,66 135,-145-243,22 49,21 56,-6-15,141 263,-115-247,65 99,-103-169,1 0,2-3,45 42,-39-47,2-1,1-2,1-1,1-2,80 33,-66-39,1-1,0-2,1-4,2-1,-2-3,90-1,-111-5,-2-2,1-1,0-2,-1-1,0-1,64-23,-71 20,0-1,-1-1,-1-2,-1 0,0-2,0 0,-2-1,35-36,57-55,-23 24,29-59,-33 37,-67 84,287-339,-169 188,33-43,111-143,-182 237,119-128,-184 221,0 0,1 1,3 3,47-25,-52 32,1 1,1 2,1 0,-1 3,47-10,-69 19,-1 1,2 0,-2 0,2 2,-2 0,2 0,-2 1,2 1,-2 0,1 1,-1 0,1 1,-1 0,0 1,0 1,0 0,-2 0,14 10,10 11,-1 1,-3 2,0 2,-2 1,-1 1,40 63,108 238,-148-276,106 259,-83-215,30 74,106 201,-62-139,-120-227,123 233,-102-201,2-1,3-2,50 55,-32-47,77 86,-109-114,-1 2,0-1,-3 3,20 43,182 422,6-86,-195-365,63 69,-68-83,2 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6576.03">2759 3611,'2'-19,"2"-1,0 0,2 1,1-1,0 1,1 1,2-1,10-17,-11 22,-4 3,1-1,0 1,2-1,-1 0,0 1,19-19,-25 30,0-1,0 0,-1 0,1 0,0 1,0-1,0 1,1-1,-1 1,0-1,0 1,0-1,0 1,0 0,0 0,1-1,-1 1,0 0,0 0,0 0,0 0,0 0,0 0,0 1,0-1,1 0,-1 1,0-1,1 1,2 1,-2 0,0 0,1 0,-1 0,0 1,0-1,0 1,-1-1,1 1,2 4,3 6,-2 2,0-1,4 20,1 20,-4 1,-1 68,-4-74,1-1,4 1,14 67,-12-92</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7854.99">4739 4488,'0'-3,"1"-1,0 0,0 0,0 1,1 0,-1-1,1 0,0 1,1-1,-1 1,1 0,-1 0,1 0,-1 0,1 0,0 1,0 0,1 0,6-4,-3 1,1 0,2 1,-2 0,0 0,2 1,-1 0,12-1,-19 4,0 0,1 0,-1 0,0 0,0 0,1 1,0-1,-1 1,0-1,0 0,0 1,0 0,0 0,0 0,0 0,0 0,-1 1,1-1,1 1,-2-1,1 1,-1 0,1-1,-1 1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,-1 0,1 0,-1 0,1 3,2 11,-1-1,-1 0,0 27,-1-37,0 2,1 0,-2-1,1 1,-1 0,0 0,0 0,-1 0,0-1,0 0,0 1,-1-1,0 1,0-1,-1-1,-1 1,1-1,0 1,-1-1,0 0,-1 0,1 0,-1-2,-11 8,17-10,0-1,-1 0,1 0,-1 0,1 0,-1 0,1 1,0-1,-1 0,1 0,-1 1,1-1,0 0,-1 1,1-1,0 0,-1 1,1-1,0 0,0 1,-1-1,1 1,0-1,0 0,0 1,-1-1,1 1,0-1,0 1,0-1,0 1,0-1,0 1,0-1,0 1,19 7,51-1,-40-5,235 48,-224-43</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9326">8205 2089,'105'-1,"113"2,-194 1,0 0,-1 2,-1 1,1 1,0 0,42 18,-62-22,0-1,-1 0,1 1,0 0,-1 0,1-1,-1 1,1 1,-1-1,0 0,0 1,0-1,0 1,0-2,-1 2,1 0,-1 0,0 0,0 0,0 0,0 0,-1 0,1 0,-1 0,0 0,1 0,-2 0,1-1,0 1,-1 1,1-1,-1 0,-1 4,-1 1,0-1,-1-1,1 1,-1-1,-2 1,2-1,-1 0,0-1,-1 1,0-1,0 1,-9 5,-1-2,11-7,0 1,-1 0,1 1,1-1,-1 1,1 0,-6 6,10-9,-1 0,1-1,-1 1,1 0,0 0,-1 0,1-1,0 0,0 1,0 0,0 0,-1 0,1 0,0 0,1 0,-1 0,0 0,0-1,0 1,1 2,0-1,0 0,1 0,-1-1,0 1,2 0,-2-1,1 1,0-1,0 1,-1-1,1 0,3 2,77 36,-62-32,0 1,-2 2,1 0,0 0,-2 2,19 15,-32-22,0 0,-1 0,0 1,1-1,-1 1,0-1,-1 1,0 0,0 0,-1 0,0 0,0 1,0-2,-1 1,0 1,0-1,0 0,-2 7,0-3,1 0,-2 0,1-1,-1 1,-1-1,-1 0,1 0,-1 0,0-1,-10 14,5-13,1 1,-2-1,0 0,-1-1,1 0,-1-1,0 0,-2 0,2-2,-2 0,-17 5,6-3,-1-2,-1-1,1-1,-1-1,-31-1,34-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11194.99">9991 516,'-34'2,"1"1,0 2,-1 0,1 2,1 2,-40 14,52-17,0 2,0 0,-29 16,42-19,1 0,-1 0,1 0,0 1,0-1,0 1,1 0,0 1,1 0,0 0,0-1,-5 11,-1 15,-1 1,4 0,0 2,3-2,0 1,4 61,0-86,0 0,1-1,1 1,0-1,0 1,0-1,1 1,0-2,1 1,0 0,1 0,5 7,-1-4,1-1,-1 1,1-3,1 2,0-1,1-1,13 8,5 0,0-2,0-1,2-1,0-2,62 13,-88-22,1 1,-1-1,0 0,0 0,1-1,-1 0,0 0,1 0,0-1,-1 1,0-2,0 1,-1-1,2 1,-1-2,0 1,-1-1,1 0,0 0,-1 1,0-2,-1 1,2-1,-1-1,-1 1,0 0,0-1,6-7,12-18,22-24,49-82,-83 118,-1-1,1 0,-2-1,-2 0,0 0,0 0,-1-1,1-39,-10-133,4 190,0 1,-1-1,1 1,-1-1,0 1,0-1,1 1,-1 0,-1-1,1 1,0 0,-1 1,0-1,0 0,1 0,-1 0,0 0,0 0,0 1,0-1,0 1,0 0,-3-2,-2 1,0 0,1 0,-1 0,0 1,0 0,0 0,-11 0,-8 2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12224">10487 1160,'0'5,"0"6,0 13,0 17,-5 5,-1 0,0-4,0-5,9-9,10-21,9-22,5-12,7-11,-2-2,-1 5,-2 8,-6 9</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12935">11807 412,'-2'11,"1"0,-1 0,-1-1,0 1,0-1,-1 0,-1 0,-6 10,1-1,-148 278,-47 96,201-384,-1 2,2-1,-2 1,2-1,1 1,0 0,-1 16,3-23,1-1,-1 0,1 1,0-1,0 0,0-1,0 1,0 0,1 0,0 0,-1 0,2 0,-1-1,0 1,0 0,1-1,-1 0,1 0,-1 1,1-2,0 1,1-1,-1 1,0-1,0 0,0 1,0-1,0 0,6 0,33 8,1-1,0-3,1-1,71-3,-90-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13522.02">12110 232,'-5'96,"-35"177,18-155,-136 565,40-208,53-17,63-439,-1 11</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7072,37 +7072,37 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">2091 0,'3'74,"4"0,3-1,20 76,125 444,9 40,13 488,-93-515,178 928,-146-809,-58 5,-56-528,10 237,-9-409</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1071.99">1 4789,'1'-1,"0"-1,0 0,0 1,1-1,-1 1,1-1,-1 1,1-1,0 1,-1 0,1 0,0 0,0 0,0 0,0 0,0 1,0-1,0 1,0-1,0 1,0 0,2 0,9-4,68-21,2 3,0 4,2 4,138-6,1089 10,-867 12,4870 0,-5290-1,0-1,0-2,0 0,0-2,0 0,44-16,-42 13,-1 1,1 1,0 1,0 1,1 2,46 3,-25-2,56 1,183-25,-243 12,-29 5</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1658.99">4075 3307,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2704">7118 1402,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3480.99">3917 1878,'4'0,"20"0,6 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3808.99">5478 2804,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4144">5636 1905,'0'-4,"0"-16,0-3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4476.99">5636 1085,'4'0,"16"0,3 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4821.99">6562 1640,'9'14,"3"18,4 16,-1 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5186">6986 3043,'0'5,"0"1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6688.99">4208 4392,'-4'1,"1"-1,0 1,0 0,0-1,-1 1,1 1,0-1,0 0,1 1,-1-1,0 1,0 0,1 0,-1 0,1 1,0-1,-1 0,1 1,0-1,0 1,1 0,-1 0,1 0,-1 0,1 0,0 0,0 0,0 0,0 5,-4 13,2-1,0 1,1 29,1-39,5 332,-3-333,1 0,1 1,0-2,0 1,1 0,0-1,0 1,7 9,53 71,-44-64,-16-20,12 17,1-2,0 0,2-1,28 25,-24-29</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8413">7991 4286,'2'4,"0"-1,-1 0,1 1,0-1,-1 1,0-1,0 1,0 0,0-1,-1 1,1 0,-1 5,1 3,8 72,-4 0,-8 116,-2-168,-2 0,0-1,-2 0,-1 0,-2-1,-1-1,-25 43,15-21,16-29</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12977">2038 5053,'0'5,"0"10,0 25,0 20,0 17,0 13,0 6,0 17,0-1,0-11,0-13,0-22</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14673">2038 5159,'3'0,"0"-2,0 1,0 0,0 0,0-1,-1 0,1 0,0 1,3-5,14-8,-7 9,-1 1,1 0,0 1,0 0,0 1,17-1,85 3,-61 2,-46-2,79 4,-79-3,1 0,-1 0,0 1,0 0,0 1,-1 0,1 0,8 5,-15-8,-1 0,1 1,0-1,-1 0,1 1,0-1,-1 1,1-1,-1 1,1-1,-1 1,1-1,-1 1,1 0,-1-1,1 1,-1 0,0-1,1 1,-1 0,0-1,0 1,1 0,-1 0,0-1,0 1,0 0,0 0,0-1,0 1,0 0,0 0,0-1,-1 2,0 0,-1 0,1-1,-1 1,1 0,-1-1,0 0,0 1,0-1,0 0,0 0,-3 2,-62 17,66-19,-75 13,42-9,-53 17,58-14,-45 6,57-12,0 1,0 0,0 1,0 1,1 1,0 0,-28 16,31-9,11-3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16902.12">8970 4921,'-14'407,"1"-48,13-292,-2 1,-4-1,-23 112,23-157</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18108.12">8864 5477,'1'-44,"2"0,3-1,1 2,2-1,2 1,2 0,2 1,33-67,-45 104,0-1,1 1,0 0,0 0,0 1,0-1,1 1,-1 0,1 0,0 0,1 1,-1-1,1 1,-1 1,1-1,0 1,0 0,0 0,0 1,7-1,13-1,0 1,0 1,43 5,-14-1,-47-3,0 1,-1 0,1 0,-1 0,1 1,-1 0,1 1,-1 0,0 0,0 0,0 1,-1 0,1 0,-1 1,0-1,8 9,-6-3,0 0,0 0,-1 1,-1 0,0 0,0 1,-1 0,-1 0,4 13,2 10</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18959.13">8997 5344,'4'0,"7"0,9 0,11 0,9 0,7 0,0 0,-4 0,0 0,2 0,-3 0,-3 0,-5 0,-7 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="38800.01">3970 3307,'9'5,"1"-1,0 0,0-1,0-1,1 1,-1-1,0-1,1 0,0-1,-1 0,18-2,-25 2,1-1,-1 1,1-1,-1 0,0 0,1 0,-1 0,0-1,0 1,0-1,0 0,0 0,0 0,0 0,-1-1,1 1,-1-1,1 1,-1-1,0 0,0 0,0 0,-1 0,1 0,-1 0,0-1,0 1,0 0,0-1,0 1,-1-1,1 1,-1-1,0 1,0-1,-1 1,0-6,0 6,1 0,-1 0,0 0,-1 0,1 0,0 0,-1 0,1 1,-1-1,0 0,0 1,0 0,0-1,-1 1,1 0,-1 0,1 0,-1 0,0 1,1-1,-1 1,0 0,0-1,0 1,0 1,0-1,0 0,0 1,-1-1,1 1,-4 0,1 0,0 0,0 0,0 0,0 1,0 0,0 0,0 0,0 1,0 0,1 0,-1 0,1 1,0 0,-1 0,-7 7,5-3,2 1,-1 0,1 0,1 1,-8 14,12-20,0-1,0 1,0 0,0 0,0-1,1 1,-1 0,1 0,0 0,0 5,0-6,1-1,-1 0,1 1,-1-1,1 0,-1 1,1-1,0 0,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0-1,1 1,-1 0,0-1,0 1,0-1,2 1,29 6,5-3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="39923.01">4710 2408,'-9'1,"1"0,-1 0,1 1,0 0,0 0,0 1,0 0,0 1,1-1,-1 1,1 1,0 0,0 0,1 0,0 0,0 1,0 0,0 1,1-1,0 1,-5 9,5-9,1 1,0 0,1-1,-1 1,2 0,-1 0,1 1,0-1,1 1,0-1,0 1,1-1,0 1,0-1,1 1,0-1,1 1,0-1,0 0,0 0,6 11,-5-14,1-1,-1 1,1 0,0-1,0 0,1 0,-1 0,1 0,0-1,0 0,0 0,1 0,-1-1,0 0,1 0,0 0,0 0,-1-1,1 0,0 0,0-1,0 0,9 0,-10 0,1 0,-1-1,0 1,0-1,1 0,-1-1,0 1,0-1,0 0,0 0,0 0,-1-1,1 0,-1 0,0 0,1 0,-1-1,-1 1,1-1,0 0,-1 0,0-1,0 1,0-1,-1 1,3-6,10-49,15-113,-25 130,3-37,-6 43</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="41043.01">5054 3175,'-1'92,"2"105,-1-193,1 0,-1 1,1-1,0 1,0-1,0 0,1 0,-1 0,1 1,0-1,0-1,0 1,1 0,0-1,-1 1,1-1,0 0,5 4,-2-3,-1 0,1-1,0 0,0-1,0 1,1-1,-1 0,1 0,-1-1,1 0,9 0,-14-1,1 1,-1-1,0 0,1-1,-1 1,0 0,0-1,1 1,-1-1,0 0,0 0,0 1,0-2,0 1,0 0,0 0,0 0,0-1,-1 1,3-3,-2 1,1-1,-1 0,0 0,0 0,0 0,0 0,-1 0,1 0,1-9,-1-8,0-1,-2 0,-2-32,1 33,-7-33,2 36</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="41991.01">5795 2355,'-9'0,"0"0,0 0,-1 0,1 1,0 0,0 0,-16 5,23-4,-1-1,0 1,0 0,0 0,1 0,-1 0,1 1,0-1,0 1,0-1,0 1,0 0,0-1,1 1,-1 0,1 0,0 1,0-1,0 0,0 0,0 0,0 5,-2 13,0 0,2 0,0 0,3 35,-2-51,1 1,-1-1,1 0,0 0,0 1,1-1,0 0,-1 0,2-1,-1 1,1 0,-1-1,1 1,0-1,1 0,-1 0,1 0,0 0,0-1,0 1,0-1,1 0,6 3,-10-5,1-1,-1 0,0 0,1 1,-1-1,0 0,0 0,1 0,-1 0,0 0,1 0,-1-1,0 1,1 0,-1-1,0 1,0-1,0 1,1-1,-1 0,0 1,0-1,0 0,0 0,0 0,0 0,0 0,0 0,-1 0,1 0,0 0,-1 0,1 0,0-1,-1 1,0 0,1 0,-1-1,0 1,1 0,-1-3,2-8,0 0,-1 0,1-18,-2 22,0-29,-1 3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="42911.01">6166 3201,'-2'1,"0"-1,0 1,0 0,0-1,0 1,0 0,1 0,-1 0,0 1,1-1,-1 0,1 0,-1 1,1-1,0 1,-1-1,1 1,0 0,-1 2,-19 36,19-37,-3 11,-1 1,2-1,0 1,0 0,2 0,0 0,0 0,2 0,1 20,-1-29,0 0,1 0,0 0,0 0,0-1,1 1,0 0,0-1,0 0,1 1,0-1,0 0,0 0,1-1,-1 1,1-1,0 1,0-1,1 0,-1-1,1 1,0-1,0 0,0 0,1 0,7 2,-5-3,0 1,-1-2,1 1,0-1,1 0,-1-1,0 0,0 0,15-3,-20 3,0-1,0 0,0-1,0 1,0-1,0 1,0-1,-1 0,1 0,0 0,-1 0,0 0,1-1,-1 1,0-1,0 1,0-1,-1 0,1 0,-1 0,1 0,-1 0,0 0,0 0,-1-1,2-4,0-1,-1 0,1-1,-2 1,1-1,-1 1,-1-1,1 1,-2-1,1 1,-1 0,-1 0,0 0,0 0,-1 0,-7-13,-7 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="44038.01">7250 2117,'-4'1,"1"0,0 0,0 0,0 0,0 1,0-1,0 1,0 0,0 0,0 0,1 0,-1 0,1 0,-5 6,-27 38,26-31,1 0,1 0,0 0,0 1,2 0,0 0,1 0,-2 31,4-41,1-1,0 1,0 0,1 0,-1-1,1 1,0 0,1-1,0 1,-1-1,2 0,-1 1,1-1,-1 0,1 0,1-1,-1 1,1-1,0 1,0-1,0 0,0-1,1 1,-1-1,1 0,0 0,0 0,8 3,-10-5,0 0,0 0,-1 0,1 0,0-1,0 1,0-1,0 1,0-1,0 0,0 0,0-1,0 1,0-1,0 1,-1-1,1 0,0 0,0 0,-1 0,5-3,-4 1,0 0,-1 0,1 0,-1 0,1 0,-1-1,0 1,0-1,0 0,-1 0,1 1,-1-1,2-7,0-13,0-1,-1 1,-2-1,-2-28,1 35,0-9,0 3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="45099.04">7171 3122,'-2'112,"-1"-38,12 119,-8-187,0 0,0 0,1-1,-1 1,1 0,1 0,-1-1,1 0,0 1,0-1,0 0,1 0,0-1,0 1,7 6,-2-5,0 0,-1-1,2 0,-1 0,1-1,-1 0,1-1,13 3,-19-5,-1 0,0 0,1 0,-1 0,1-1,-1 1,1-1,-1 0,1 0,0 0,-1-1,1 1,-1-1,1 0,-1 0,0 0,1-1,-1 1,0-1,0 1,0-1,0 0,0 0,0-1,-1 1,1 0,-1-1,1 0,-1 0,0 1,0-1,0 0,-1-1,1 1,-1 0,1 0,-1-1,0 1,0-5,4-15,-2 0,-1 0,-1 0,-3-45,0 36,3 20,-1 0,-1 0,0-1,-1 1,0 0,-1 0,0 0,-1 1,0-1,-1 1,0 0,-1 0,0 0,-1 1,-16-19,-1 7</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="47147.01">8071 1852,'-3'1,"1"-1,0 1,0-1,0 1,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 1,0-1,1 1,-1-1,1 1,0 0,-1 0,1-1,0 1,0 0,0 0,0 0,0 0,1 0,-1 0,1 0,-1 1,1 1,-4 12,2 0,-2 29,4-36,-2 20,-1-11,2-1,0 1,1-1,1 1,1-1,0 1,1-1,6 18,-9-33,1 0,-1-1,1 1,-1-1,1 1,0-1,0 1,0-1,0 1,0-1,0 0,0 1,0-1,0 0,1 0,-1 0,0 0,1 0,-1 0,1 0,-1-1,1 1,0 0,1 0,-1-2,0 1,0 0,0-1,0 0,-1 1,1-1,0 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,-1-1,0 1,1-1,1-2,4-7,0 0,0 0,-2 0,10-25,-6 1,-3-1,0 0,-3 0,0 0,-3-1,-4-38,3 30,0 30</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="51914.01">9552 2699,'-1'-1,"1"0,-1 0,0 0,1-1,-1 1,0 0,0 0,0 0,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 1,-1-1,1 1,0-1,0 1,-1-1,1 1,0 0,-1 0,1 0,-3 0,-38-4,30 4,0 0,1 1,-1 0,1 1,0 0,-1 1,1 0,0 0,1 2,-1-1,1 1,0 1,0 0,0 0,1 1,0 0,0 1,1 0,0 0,0 1,1 0,0 0,0 1,1 0,1 0,0 0,0 1,1 0,0 0,1 0,0 0,1 0,0 1,1-1,0 1,1-1,1 14,0-18,1 0,0 0,1 0,-1-1,1 1,0-1,1 0,-1 0,1 0,1 0,-1-1,1 0,0 0,9 8,10 6,1-1,30 16,-30-19,0 1,0-1,1-2,0 0,49 15,-73-28,0 1,1-1,-1 0,0 1,0-1,0 0,1-1,-1 1,0 0,0-1,0 1,1-1,-1 1,0-1,0 0,0 0,0 0,0 0,-1-1,1 1,0 0,0-1,-1 1,1-1,-1 0,0 1,1-1,-1 0,0 0,0 0,0 0,0 0,0 0,0 0,-1 0,1 0,-1 0,0-1,1-2,2-11,-2-1,1 0,-2 0,-1-18,0 22,-5-241,2 228,-2 4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="53133.01">10505 2725,'-26'0,"0"0,0 2,1 0,-39 10,56-10,-1 1,1 1,0-1,0 1,1 1,-1-1,1 1,0 1,0-1,1 1,0 0,0 1,0-1,1 1,0 0,0 1,-4 7,3-1,0 1,1-1,0 1,1 0,1 0,0 1,1-1,1 18,7 128,-5-140,0-14,-1 0,1 0,0 0,1 1,0-1,0 0,0-1,1 1,0 0,0-1,1 0,0 1,0-1,6 6,-5-7,1 0,1 0,-1-1,1 0,0 0,0 0,0-1,0 0,0-1,1 0,-1 0,1 0,8 0,-3 1,0-2,-1 1,1-2,0 1,0-2,-1 0,14-2,-21 1,0 0,0 1,0-2,0 1,-1 0,1-1,-1 0,0 0,0 0,0-1,0 1,0-1,-1 0,1 0,-1-1,0 1,-1 0,1-1,2-7,3-5,-2-1,0 0,-2-1,0 1,0-1,0-31,-7-120,0 66,2 52,1 30</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="54546.01">11113 2725,'0'0,"0"-1,-1 0,1 1,0-1,0 0,0 1,0-1,-1 0,1 1,0-1,-1 1,1-1,0 0,-1 1,1-1,-1 1,1-1,-1 1,1-1,-1 1,1-1,-1 1,1 0,-1-1,0 1,1 0,-1 0,1-1,-1 1,0 0,1 0,-1 0,0 0,0 0,1 0,-1 0,0 0,1 0,-1 0,0 0,1 0,-1 0,0 1,1-1,-1 0,1 0,-2 1,-31 15,22-6,1-1,0 2,1-1,0 1,0 1,1-1,1 1,0 1,1 0,0 0,1 0,-6 22,4-4,1 0,1 0,2 0,2 50,0-67,2-1,0 0,0 0,1 1,1-1,0 0,5 13,-4-19,-1-1,1 0,0 0,0-1,0 1,1-1,0 0,0 0,0-1,1 1,0-1,-1 0,1-1,1 0,8 4,-10-4,0-1,1 0,-1 0,0 0,1-1,0 1,-1-1,1-1,0 1,0-1,-1 0,1 0,0-1,-1 0,1 0,6-2,-6 1,0-1,0-1,0 1,0-1,-1 0,0-1,1 1,-1-1,-1 0,1 0,-1 0,0-1,4-7,-1 1,-1 0,0 0,-1 0,-1-1,0 0,0 0,-2 0,1 0,0-16,-2-18,-4-60,0 32,2 73,2-5,-1 0,-1 0,0 0,0 0,0 0,-3-8,3 13,0 1,1 0,-1-1,0 1,0 0,0-1,0 1,0 0,0 0,0 0,-1 0,1 0,0 0,-1 0,1 0,-1 0,1 1,0-1,-1 0,0 1,1 0,-1-1,1 1,-1 0,0 0,1 0,-1 0,1 0,-1 0,0 0,1 0,-1 1,-1 0,-3 1,0 0,0 0,0 1,1 0,-1 0,1 1,0-1,0 1,0 0,0 0,1 1,-6 7,-25 30</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="442292.54">5689 8361,'0'-30,"1"14,-1-1,0 1,-4-23,3 35,0 0,0 1,0-1,0 0,-1 0,1 1,-1-1,0 1,0-1,0 1,-1 0,1 0,-1 0,0 0,0 0,0 0,0 1,-7-4,-2 0,0 2,-1 0,1 0,-1 1,0 0,-1 2,1-1,0 1,-21 2,-124 17,146-16,-72 12,-84 26,135-31,1 2,0 2,1 1,0 1,-43 29,48-22,1 2,1 0,1 1,2 2,-21 31,-7 7,14-20,2 1,2 2,-37 76,55-95,1 2,1 0,1 0,2 1,1 0,2 0,-2 49,7-70,-1 7,0 1,2 0,0 0,2-1,4 21,-6-34,1 0,0-1,0 1,0-1,0 0,1 1,0-1,0 0,0 0,0-1,0 1,1-1,0 1,-1-1,1 0,1-1,-1 1,0-1,1 1,-1-1,1-1,-1 1,1-1,7 2,33 3,0-2,1-2,70-6,-25 1,75 4,152-5,-301 2,0 0,0 0,0-2,-1 0,1-1,-1-1,0 0,-1-1,1-1,-2 0,1-1,-1-1,0 0,-1-1,0 0,-1-1,21-26,-21 23,96-126,-97 124,0-1,-2 0,0 0,-1-1,-1 0,8-34,5-58,-4-1,0-159,-16 261,0 1,-1-1,0 0,0 0,-1 0,-1 1,-5-17,5 21,0 0,0-1,0 1,-1 1,1-1,-1 0,0 1,-1 0,1 0,-1 0,0 1,0-1,0 1,-8-4,-40-18,-100-35,122 52,0 0,0 2,0 1,-1 2,-37 1,30 2,4 2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="443291.56">6377 8070,'4'0,"7"0,9-9,7-3,8 1,6 2,10 2,10 3,12-3,3 0,7-3,16-9,31-6,8 2,-15 4,-30 1,-24 4,-26 4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="444726.55">7832 7620,'1'-5,"1"0,0 0,1 0,-1 1,1-1,0 1,0-1,7-7,-2 2,147-179,-84 107,61-94,-130 173,-1 0,1 0,0 0,0 1,0-1,0 1,0-1,1 1,-1 0,1 0,-1 0,1 0,0 0,0 1,4-2,-6 3,-1 0,1 0,0 0,0 0,-1 0,1 0,0 0,0 0,-1 1,1-1,0 0,0 1,-1-1,1 0,0 1,-1-1,1 1,-1-1,1 1,-1-1,1 1,0 1,12 29,-5 14,-2 0,-2 1,-2-1,-7 77,2-60,8 103,15 21,-19-159</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">2177 0,'3'72,"4"0,4-1,20 74,130 433,10 38,13 475,-96-501,184 904,-151-789,-60 6,-59-514,10 230,-9-398</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1071.99">1 4662,'1'-1,"0"-1,0 0,0 1,1 0,-1 0,1-1,-1 1,1-1,1 1,-2 0,1 0,0 0,0 0,0 0,0 0,0 1,0-1,0 1,0-1,0 1,1 0,1 0,9-4,72-20,1 2,0 5,3 3,143-5,1134 9,-903 12,5070 0,-5507-1,0-1,0-2,0 0,0-2,1 0,44-15,-43 12,0 1,0 1,0 1,0 1,1 2,48 3,-26-2,58 1,191-24,-253 11,-30 5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1658.99">4242 3220,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2704">7410 1365,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3480.99">4078 1828,'4'0,"21"0,6 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3808.99">5703 2730,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4144">5867 1855,'0'-4,"0"-16,0-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4476.99">5867 1056,'5'0,"15"0,4 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4821.99">6831 1597,'10'13,"2"18,5 16,-1 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5186">7273 2963,'0'4,"0"2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6688.99">4381 4276,'-4'1,"0"-1,1 1,0 0,0-1,-1 1,1 1,0-1,0 0,0 1,0-1,0 0,0 1,1 0,-1 0,1 1,0-1,-1 0,1 1,-1-1,1 1,1 0,-1 0,1 0,-1 0,1 0,0-1,0 1,0 0,0 5,-4 13,2-2,-1 1,2 29,1-38,5 323,-2-325,0 1,1 1,0-2,0 0,1 1,0-1,0 1,8 8,55 70,-47-63,-15-19,11 16,2-1,0-1,1 0,30 24,-25-29</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8413">8319 4173,'2'4,"0"-2,-1 1,1 1,0-1,-1 1,0-1,1 1,-1 0,0-1,-1 1,1-1,-1 6,1 3,8 70,-4-1,-8 114,-2-164,-2 1,-1-2,-1 0,-1 0,-3-1,0-1,-27 43,16-22,17-27</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12977">2122 4919,'0'5,"0"10,0 24,0 19,0 17,0 13,0 5,0 17,0-1,0-10,0-14,0-20</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14673">2122 5023,'3'0,"0"-2,0 1,0 0,0 0,0-1,-1 0,2 0,-1 1,3-5,15-8,-8 10,0 0,0 0,1 1,-1 0,1 1,17-1,89 3,-64 2,-48-2,83 4,-83-3,2 0,-2 0,0 1,1 0,-1 1,-1 0,2-1,7 6,-15-8,-1 0,1 1,0-1,-1 0,1 1,0-1,-1 1,2-1,-2 1,1-1,-1 1,1-1,-1 1,1 0,-1-1,1 1,-1 0,0-1,1 1,-1 0,0-1,0 1,1 0,-1 0,0-1,0 1,0 0,0 0,0-1,0 1,0 0,0 0,0-1,-1 2,0 0,-1 0,1-1,-2 0,2 1,-1-1,0 0,0 1,0-1,0 0,0 0,-3 2,-65 17,69-19,-78 12,43-8,-54 17,60-15,-47 7,59-12,0 1,1 0,-1 1,0 0,1 2,1 0,-30 16,32-10,12-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16902.12">9338 4791,'-14'396,"0"-46,14-285,-2 1,-4-1,-24 109,23-152</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18108.12">9228 5332,'1'-43,"2"0,3 0,2 1,1-1,2 1,3 0,2 1,34-65,-47 101,0 0,1 0,0 0,0 0,0 1,1-1,0 1,-1 0,1 0,0 1,2 0,-2-1,1 1,-1 1,2-1,-1 1,0 0,0 0,0 1,8-1,13-1,0 1,0 1,45 5,-15-1,-48-3,-1 1,-1 0,2 0,-2 0,1 1,0 0,0 1,-1 0,0 0,1 0,-1 1,-1-1,2 1,-2 1,0-1,9 9,-7-4,0 1,1 0,-2 1,-1-1,0 1,1 1,-2-1,-1 1,4 12,3 11</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18959.12">9366 5203,'5'0,"6"0,10 0,11 0,10 0,7 0,0 0,-5 0,1 0,2 0,-3 0,-4 0,-4 0,-8 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="38800.01">4133 3220,'9'4,"2"0,-1 0,1-1,-1-1,1 1,0-1,-1-1,2 0,-1-1,0 0,18-2,-26 2,1-1,-1 1,1-1,-1 0,1 0,0 0,-1 0,0-1,0 1,0-1,0 0,0 0,1 0,-1 0,-1 0,1 0,-1-1,1 1,-1-1,0 0,0 0,0 0,-1 0,2 0,-2 0,0-1,0 1,0 1,0-2,0 1,-1-1,1 1,-1-1,0 1,0-1,-1 1,0-6,0 7,1-1,-1 0,0 0,-1 0,0 0,1 0,-1 0,1 1,-1-1,0 0,0 1,0 0,0 0,-1 0,1 0,-1 0,1 0,-2 0,1 1,1-1,-1 1,0 0,0-1,0 1,0 1,-1-1,1 0,0 1,-1-1,1 1,-4 0,0 0,1 0,0 0,0 0,-1 1,1 0,0 0,0 0,-1 1,1 0,1 0,-1 0,0 1,1 0,-1 0,-7 6,4-2,3 1,-1 0,0-1,2 2,-8 14,12-20,0-2,0 2,-1 0,1 0,0-1,1 1,-1 0,1 0,0 0,0 5,0-6,1-1,-1 0,1 0,-1 0,1 0,-1 1,2-1,-1 0,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0-1,1 1,-1 0,0-1,0 1,0-1,2 1,31 6,4-3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="39923.01">4903 2344,'-9'1,"1"0,-2 0,2 1,0 0,-1 0,1 1,0 0,-1 1,2-1,-1 1,0 0,1 1,0 0,1 0,-1 0,1 1,0 0,0 0,0 0,1 1,-5 9,5-9,0 0,1 1,1-1,-1 1,2-1,-1 1,1 1,0-1,1 1,-1-2,1 2,1-1,0 1,0-2,1 2,1-1,0 1,0-1,0-1,0 1,6 11,-5-14,1-2,0 2,0 0,0-1,0 0,1 0,-1 0,2 0,-1-1,0-1,0 1,2 0,-2-1,0 0,1 0,0 0,1 0,-2-1,1 0,0 0,1-1,-1 0,9 0,-9 0,0 0,-1-1,0 1,1-1,0 0,-1-1,0 1,0-1,1 0,-1 0,0 0,-1-1,1 0,0 1,-1-1,1 0,-1-1,-1 1,1-1,1 0,-2 0,0-1,0 1,0 0,-1 0,3-6,11-47,15-111,-26 127,4-36,-7 42</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="41043.01">5261 3091,'-1'90,"2"101,-1-187,1 0,-1 1,2-1,-1 1,0-1,0 0,1-1,-1 1,1 1,0-1,0-1,0 1,1 0,0-1,-1 1,2-1,-1-1,5 5,-2-3,-1 0,2-1,-1 0,0-1,0 1,2-1,-2 0,1 0,0-1,0 0,9 0,-13-1,0 1,-1-1,0 0,1-1,-1 1,0 0,0-1,1 1,-1-1,0 0,1 0,-1 1,0-2,0 1,0 0,0 0,0 0,0-1,-1 1,3-3,-2 1,2-1,-2 0,0 0,0 1,0-1,0 0,-1 0,1 0,1-9,-1-7,0-2,-2 1,-2-32,1 33,-7-33,2 36</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="41991.01">6033 2293,'-9'0,"-1"0,1 0,-2 0,2 1,0 0,-1 0,-16 4,24-3,-1-1,0 1,0 0,0 0,1 0,-2 0,2 1,0-1,0 1,0-1,0 1,0 0,0-1,1 1,-1-1,1 1,0 1,0-1,0 0,0 0,-1 0,1 5,-2 12,0 1,2-1,0 1,3 33,-2-49,1 1,-1-1,1 0,0-1,0 2,1-1,1 0,-2 0,2-1,-1 1,1-1,-1 0,1 1,0-1,1 0,0 0,0 0,0 0,0-1,0 1,0-2,2 1,5 3,-10-5,1-1,-1 0,0 0,1 1,-1-1,0 0,0 0,1 0,0 0,-1 0,1 0,-1-1,0 1,1 0,-1-1,0 1,0-1,0 1,1-1,-1 0,0 1,0-1,0 0,0 0,0 0,0 0,0 0,0 0,-1 0,1 1,1-1,-2 0,1 0,0-1,-1 1,0 0,1 0,-1-1,0 1,1 0,-1-3,2-8,0 1,-1-1,1-17,-2 21,0-28,-1 3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="42911.01">6419 3116,'-2'1,"0"-1,0 1,0 0,0-1,0 1,0 0,0 0,0 0,0 1,1-1,-1 0,1 0,-1 1,1-1,0 1,-1-1,1 1,0 0,-1 2,-20 35,20-36,-3 10,-2 2,3-2,0 2,0 0,2-1,0 1,0-1,2 1,1 19,-1-28,0 0,1 0,0-1,0 1,0-1,1 1,0 0,0-1,0 0,1 0,0 0,1 0,-1 0,1-1,-1 1,1-1,0 1,0-2,2 1,-2-1,1 1,0-1,0 0,1 0,0 0,7 2,-4-3,-1 1,-1-2,2 0,-1 0,1 0,0-1,-1 0,0 0,16-3,-21 3,1 0,-1-1,0-1,0 1,0-1,0 1,0-1,-1 0,1 0,1 0,-2 0,0 0,1-1,-1 1,0-1,0 1,0-1,-1 0,1 1,-1-1,1 0,0 0,-1 0,0 0,-1-1,2-4,0-1,-1 1,1-2,-2 1,1-1,-1 2,-1-2,1 1,-2-1,1 2,-1-1,-1 0,-1 0,1 1,-1-1,-7-13,-8 2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="44038.01">7548 2061,'-5'1,"2"0,0 0,0 0,0 0,0 1,0-1,0 1,-1 0,1 0,0 0,1 0,-1-1,1 1,-5 6,-29 37,28-30,1-1,0 1,1-1,0 2,2 0,0-1,0 1,-1 29,4-39,1-1,0 1,0 0,1 0,-1-1,1 0,0 1,1-1,0 1,0-1,1 0,-1 1,1-2,-1 1,1 0,1-1,-1 1,2-1,-1 1,0-1,0-1,0 0,1 1,0-1,0 0,0 0,0 0,9 3,-11-5,0 0,0 0,-1 0,1 0,0-1,1 1,-1-1,0 1,0-1,0 0,0 0,0-1,0 1,0-1,1 1,-2-1,1 0,0 0,0 0,-1 0,5-3,-3 1,-1 0,-1 0,1 0,-1 0,1 0,-1-1,0 2,0-2,0 0,-1 0,2 1,-2-1,2-7,0-12,0-1,-1 0,-2 0,-2-28,1 35,0-9,0 2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="45099.04">7465 3039,'-2'109,"-1"-36,13 114,-9-181,0 0,0 0,1-1,-1 1,1-1,1 1,-1-1,1 0,0 1,0-1,1 0,0-1,0 0,0 1,8 6,-3-5,0 0,0-1,1-1,-1 1,2-1,-2 0,2-1,12 3,-18-5,-2 0,0 0,1 0,-1 0,1-1,-1 1,2-1,-2 0,1 0,0 0,-1-1,1 1,-1-1,2 0,-2 0,0 0,1-1,-1 1,0-1,0 1,1-1,-1 0,0 0,0-1,-1 1,1 0,-1-1,1 0,-1 1,1 0,-1-1,0 0,-1-1,1 1,-1 0,1 0,-1-1,0 1,0-5,4-14,-2 0,-1-1,-1 1,-3-44,0 35,3 19,-1 0,-1 0,0 0,-1 0,0 0,-1 1,0-1,-1 1,0 0,-2 0,1 0,-1 1,0-1,-2 1,-16-18,-1 6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="47147.01">8402 1803,'-3'1,"1"-1,0 1,0-1,0 1,0 0,0 0,0 0,0 0,-1 0,1 0,1 0,-1 1,0-1,1 1,-1-1,1 1,0-1,-1 1,1-1,0 1,0 0,0 0,0 0,0 0,1 0,-1 0,1 0,-1 1,1 1,-5 11,3 1,-2 28,4-35,-2 19,-1-11,2 0,0 0,1 0,1 0,1 0,0 1,1-2,7 18,-10-32,1 0,-1-1,1 1,-1-1,1 1,0-1,0 1,0-1,0 1,0-1,0 0,0 1,0-1,0 0,1 0,-1-1,0 1,1 0,-1 0,1 0,-1-1,2 1,-1 0,1 0,-1-2,0 1,0 0,0-1,0 0,-1 1,1-1,0 0,-1 0,1 0,0 1,0-1,-1 0,1 0,-1-1,0 1,1-1,1-2,4-7,1 0,-1 1,-2-1,11-24,-7 1,-3-1,1 0,-4 0,0 0,-3-1,-4-37,3 29,0 29</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="51914.01">9944 2628,'-1'-1,"1"0,-1 0,0 0,1-1,-1 1,0 0,0 0,0 0,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 1,-2-1,2 1,0-1,0 1,-1-1,1 1,0 0,-1 0,1 0,-3 0,-40-4,32 4,-1 0,2 1,-2 0,2 1,-1 0,0 1,0 0,1 0,0 2,0-1,1 0,-1 2,1 0,-1 0,2 1,0 0,-1 0,2 1,0 0,-1 1,2-1,0 1,-1 1,2 0,1-1,0 1,0 1,0 0,1-1,1 1,0 0,1-1,0 2,1-1,0 1,1-2,1 15,0-19,1 1,0 0,1 0,-1-1,1 0,0 0,2 0,-2 0,1 0,1 0,-1-1,1-1,1 1,8 8,11 5,1 0,32 15,-32-18,0 0,0 0,1-2,0-1,51 15,-76-27,0 1,1-1,-1 0,0 1,0-1,0 0,2-1,-2 1,0 0,0-1,0 1,1-1,-1 1,0-1,0 1,0-1,0 0,1 0,-2-1,1 1,0 0,0-1,-1 1,1-1,-1 0,0 1,1-1,-1 0,0 0,0 0,0 0,0 0,0 0,0 0,-1 0,1 0,-1 0,0 0,1-3,3-11,-3 0,1-1,-2 0,-1-17,0 22,-6-236,3 223,-2 4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="53133.01">10936 2653,'-27'0,"0"0,0 2,1 0,-41 9,59-9,-1 1,0 1,1-1,0 1,0 1,0-1,1 1,0 1,-1-2,2 2,0 0,-1 1,1-1,1 1,0-1,0 2,-5 7,4-2,0 2,1-1,-1 0,2 1,1-1,0 2,1-1,1 17,7 124,-5-135,0-14,-1 0,1-1,0 1,1 1,0-1,0 0,1-2,0 2,0 0,0-1,1 0,0 1,0-2,7 7,-6-7,1 0,2 0,-2-1,1 0,0-1,1 1,-1-1,0 0,1-1,0 0,-1 0,1 0,9 0,-3 1,-1-2,0 1,0-2,1 1,-1-2,0 0,14-2,-22 1,0 0,0 1,1-2,-1 1,-1 0,1-1,-1 0,1 0,-1 0,0 0,0 0,0-1,-1 0,2 0,-2-1,0 1,-1 0,1-1,2-6,4-6,-3 0,0-1,-2 0,0 0,1 0,-1-31,-7-117,-1 65,3 51,1 28</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="54546.01">11569 2653,'0'0,"0"-1,-1 0,1 1,0-1,0 0,0 1,0-1,-1 0,1 1,0-1,-1 1,1-1,0 0,-1 1,1-1,-1 1,1-1,-1 1,1-1,-1 1,1-1,-1 1,1 0,-1-1,0 1,1 0,-1 0,1-1,-1 1,0 0,1 0,-1 0,0 0,0 0,1 0,-1 0,-1 0,2 0,-1 0,0 0,1 0,-1 0,0 1,1-1,-1 0,1 0,-2 1,-32 15,22-6,2-2,0 3,0-1,1 0,-1 2,2-1,1 1,0 0,0 1,1 0,1-1,-7 22,5-4,1 1,1-1,2 0,1 49,1-66,2 0,1 0,-1-1,1 2,1-1,0-1,5 14,-4-19,0-2,0 1,0 0,0-1,0 1,1-1,1-1,-1 1,0-1,1 1,0-1,0 0,0-1,1 0,9 4,-11-5,0 0,2 0,-2 0,0 0,1-1,0 1,0-1,0-1,0 1,0-1,0 0,0 0,0-1,-1 0,1 0,7-2,-7 1,0-1,1 0,-1 0,0-1,-1 0,1-1,0 1,-1-1,-1 0,1 0,0 1,-1-2,4-7,-1 1,0 1,-1-1,-1 0,-1 0,0-1,1 0,-3 1,1-1,0-15,-2-18,-4-58,0 31,2 71,2-5,-1 0,-1 1,0-1,0 0,0 0,-4-8,4 14,0 0,1 0,-1-1,0 1,0 0,0-1,0 1,0 0,0 0,0 0,-1 0,1 0,0 0,-1 0,1 0,-1 0,1 1,0-1,-2 0,1 1,1 0,-1-1,1 1,-1 0,0 0,1 0,-1 0,1 0,-1 0,0 0,1 0,-1 1,-2 0,-2 1,0 0,0 0,-1 1,2 0,-1 0,1 1,0-2,-1 2,1 0,0 0,1 1,-7 7,-25 29</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12795.81">5923 8140,'0'-29,"1"13,-1 0,0 0,-5-22,4 34,0 0,0 1,0-1,0 0,-1 1,1 0,-1-1,0 1,0-1,0 1,-1 0,1 0,-2 0,1 0,0 0,0 1,0 0,-7-4,-3 0,1 2,-2 0,2 0,-2 1,0 0,0 2,0-1,1 1,-23 2,-128 17,151-16,-74 12,-88 24,141-29,0 2,1 2,1 0,0 2,-45 28,49-22,2 2,1 1,1 0,3 2,-23 31,-7 6,14-19,3 1,2 2,-39 73,57-92,2 3,1-1,0 0,3 1,1 0,1 0,-1 48,7-68,-1 7,0 0,2 1,0-1,2 0,4 20,-6-34,2 1,-1-1,0 1,0-1,0 0,1 1,0-1,0-1,0 1,1-1,-1 1,1-1,0 1,-1-1,1 0,1-1,0 1,-1-1,1 1,-1-1,1-1,0 0,0 0,7 2,35 3,0-2,1-2,73-6,-27 1,79 4,158-5,-313 2,0 0,-1 0,1-1,-1-1,0-1,0-1,0 0,-2-1,2 0,-3-1,2-1,-1-1,-1 0,0 0,-1-1,0-1,21-25,-21 23,99-123,-100 120,-1-1,-2 1,1-1,-2 0,-1-1,9-32,5-57,-5-1,1-155,-17 254,0 1,-1 0,0-1,0 0,-1 0,-1 2,-6-18,6 21,0 1,0-2,0 1,-1 1,1-1,-2 0,1 1,-1 0,1 1,-1-1,0 1,-1-1,1 1,-8-4,-43-17,-103-35,127 52,0-1,-1 2,1 1,-1 2,-39 1,31 2,5 2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13794.83">6639 7857,'4'0,"7"0,10-9,7-3,9 1,5 3,12 1,9 3,13-3,3 0,8-2,16-10,32-5,9 1,-16 5,-32 0,-24 5,-27 3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15229.82">8154 7418,'1'-4,"1"-1,0 0,1 0,-1 1,1-1,0 1,0-1,8-6,-3 1,153-174,-87 104,64-91,-136 168,-1 0,1 0,0 0,0 1,0-1,0 1,0-1,1 1,0 1,0-1,-1 0,1 0,0 0,0 1,4-2,-6 3,-1 0,1 0,1 0,-1 0,-1 0,1 0,0 0,0 0,-1 1,1-1,0 0,0 1,-1-1,1 0,0 1,-1-1,1 1,-1-1,1 1,-1-1,1 1,0 1,13 28,-6 14,-2-1,-2 2,-2-1,-7 75,2-59,8 101,16 20,-20-155</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7156,10 +7156,10 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">375 32,'-2'144,"5"156,-3-293,0 0,1 0,0-1,0 1,1 0,0 0,0-1,1 0,-1 1,1-1,1 0,-1 0,1 0,5 5,-4-6,1 0,0 0,0-1,0 0,1 0,-1 0,1-1,0 0,0-1,0 1,0-1,1-1,7 2,-7-2,1 1,-1-2,1 1,0-1,-1 0,1-1,0 0,-1 0,1-1,-1 0,1-1,-1 0,0 0,0-1,11-6,-14 6,1 0,-1 0,0-1,-1 0,1 0,-1 0,0 0,0-1,-1 0,0 1,0-1,0 0,0-1,-1 1,0 0,-1-1,1 1,-1-1,0 0,-1-11,-5-407,5 423,0 0,0-1,0 1,0 0,0-1,1 1,-1 0,1-1,0 1,-1 0,1 0,0 0,0-1,1 1,-1 0,3-3,-3 5,-1-1,1 1,-1 0,1-1,0 1,-1 0,1 0,0-1,-1 1,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,0 1,-1-1,2 0,20 18,-11-3,-1-1,-1 1,-1 1,0-1,-1 2,0-1,-2 1,0 0,4 19,2 29,3 67,-13-113,7 469,-10-298,1-172,-1-1,-1 0,0 1,-1-1,-1-1,-1 1,0-1,-1 0,-1 0,0-1,-1 0,-1 0,0-1,-16 16,14-17,0 0,-1-1,0-1,0 0,-1-1,-1 0,0-1,0-1,-1 0,1-1,-2-1,1 0,-1-2,-23 5,-89 9,55-7,-106 4,169-15,1 0,-1 1,1-2,-1 0,1 0,-18-5,25 5,0 0,1 0,-1-1,0 0,0 1,1-1,-1 0,1 0,-1-1,1 1,0 0,0-1,0 1,0-1,0 0,1 0,-1 1,1-1,0 0,-1 0,2 0,-2-6,-1 2,2-1,-1 0,1 0,0 0,0 1,1-1,0 0,1 0,0 0,0 0,1 0,-1 1,2-1,-1 1,1-1,0 1,1 0,0 0,0 0,0 0,1 1,0 0,0 0,0 0,1 1,0 0,0 0,1 0,11-7,2 2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="761">1457 424,'4'0,"9"0,2-4,7-2,3-2,9-2,3 3,3 1,-1 2,-4 2,-4 1,-3 1,-2 0,-3 0,-4 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1300.99">1411 653,'8'0,"14"0,15 0,13 4,10 2,2-1,-1-1,-3-1,-8-2,-9 0,-6 0,-6-1,3 0,-2 3,-8 2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3701.99">2607 216,'16'-1,"1"-1,-1-1,-1 0,1-2,0 1,21-11,-26 10,1 0,1 0,-1 1,1 1,-1 0,1 1,0 0,0 1,0 0,0 1,14 2,-12 1,0 1,-1 0,1 1,-1 1,1 0,-2 1,1 0,-1 1,21 17,-25-18,-1 1,0 1,0-1,-1 1,0 1,0-1,-1 1,0 0,-1 1,0-1,-1 1,0 0,3 17,4 26,-3 0,-2 0,-3 1,-2-1,-9 80,5-121,0 1,-1-1,-1 1,-1-1,1-1,-2 1,0-1,0 0,-1-1,-1 1,0-2,0 1,-13 9,16-14,0 0,-1 0,1-1,-1 0,-1-1,1 1,-1-1,1-1,-1 1,0-1,0-1,-1 0,1 0,0 0,-1-1,1 0,-1-1,1 0,-1 0,0-1,1 0,-13-3,18 2,0 1,0-1,0 0,0 0,0 0,1 0,-1 0,0-1,1 1,0-1,0 0,0 0,0 0,0 0,0 0,1 0,0 0,-1 0,1-1,0 1,1 0,-1-1,1 1,-1-1,1 1,0-7,0 1,1 1,0-1,0 1,0-1,1 1,0 0,1 0,0 0,0 0,6-9,-7 14,0 1,1-1,-1 1,1 0,0-1,0 1,0 0,0 1,0-1,0 0,1 1,-1 0,0 0,1 0,-1 0,1 0,-1 1,6-1,75 3,-56-1,-13 0,1 1,-1 0,0 1,0 0,0 1,0 1,-1 0,25 14,-7 0,-1 1,42 37,-65-51,1-1,-1 1,1-1,-1-1,2 0,-1 0,0 0,1-1,-1-1,1 0,17 2,9-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">395 31,'-2'140,"5"152,-3-285,0 0,1 0,0-1,0 0,1 1,0 0,0-1,2 0,-2 0,1 0,1 0,-1 0,1 0,6 5,-5-7,1 1,1 0,-1-1,0 0,2 0,-2 0,1-1,1 0,-1-1,1 0,-1 0,1-1,8 2,-7-2,0 1,-1-2,2 1,-1-1,0 0,0-1,1 0,-2 0,2-1,-2 0,2-1,-2 1,0-1,1-1,11-6,-15 6,1 0,0 0,-1-1,-1 1,1-1,0 0,-1 0,0-1,-1 0,0 1,1 0,-1-1,0-1,-1 1,0 0,-1-1,1 2,-1-2,0 0,-1-11,-5-395,5 411,0 0,0-1,0 1,0 0,0-1,1 1,-1 0,1-1,0 1,-1 0,1 1,0-1,0-1,2 1,-2 0,3-3,-3 5,-1-1,1 1,-1 0,1-1,0 1,-1 0,1 0,0-1,-1 1,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,1 1,-2-1,2 0,21 17,-12-2,0-1,-2 0,0 2,-1-2,0 3,-1-1,-2 0,1 1,3 18,3 28,2 65,-13-109,8 456,-11-290,1-168,-1 0,-2-1,1 2,-1-2,-1 0,-2 1,1-2,-1 1,-2-1,1 0,-2-1,0 1,-1-1,-16 15,14-16,1-1,-2 0,0-1,1-1,-2 0,-1 0,0-1,1-2,-2 1,1-1,-2-1,1 0,-1-3,-24 6,-94 9,58-8,-111 5,177-15,2 0,-2 1,2-2,-2 0,2 0,-20-5,27 5,0 0,1 0,-2-1,1 0,0 1,1 0,-1-1,1 0,-1-1,0 1,1 0,0-1,0 1,0-1,0 0,1 0,-1 1,1-1,0 0,-1 0,2 1,-3-7,0 2,2-1,-1 0,1 1,0-1,0 1,1-1,0 0,1 1,0-1,0 0,1 0,-1 2,2-2,0 1,0-1,0 1,1 1,0-1,1 0,-1 0,1 1,0 0,1 1,-1-1,1 1,0 0,1 0,0 0,12-6,2 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="761">1534 413,'4'0,"10"0,2-4,7-2,3-2,10-2,3 4,3 0,-1 2,-4 2,-4 1,-4 1,-1 0,-4 0,-4 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1300.99">1486 636,'8'0,"15"0,16 0,14 3,10 3,2-1,0-1,-4-1,-9-2,-9 0,-6 0,-6-1,3 0,-3 3,-8 2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3701.99">2745 210,'17'-1,"1"-1,-1-1,-2 0,2-1,0 0,22-11,-27 10,0 0,2 1,-1 0,0 1,0 0,1 1,-1 0,1 1,0 0,-1 1,16 2,-13 1,-1 1,0 0,1 0,-1 2,0 0,-1 1,1 0,-1 1,21 16,-25-17,-2 0,1 2,-1-1,0 1,-1 1,0-2,0 2,-1 0,-1 0,0 0,0 1,-1 0,3 16,5 25,-4 1,-1 0,-4 0,-2 0,-10 77,6-117,0 0,-1 0,-1 1,-2-2,2 0,-2 1,-1-2,1 1,-2-1,0 0,-1-1,1 1,-14 8,16-13,1 0,-1 0,0-1,0-1,-1 0,0 1,0-1,1-1,-2 1,1-1,-1-1,0 0,0 0,1 0,-2-1,2 0,-1-1,0 0,0 0,-1-1,2 0,-14-3,18 2,1 1,0-1,0 0,0 0,0 0,1 0,-2 0,1-1,1 1,0-1,0 0,0 0,0 1,0-1,0 0,0 0,1 0,-1 0,1-1,0 1,1 0,-1-1,1 1,-1 0,1 0,0-7,0 1,1 1,0 0,0 0,0-1,1 1,1 0,0 1,0-1,0 0,6-8,-6 13,-1 1,1-1,-1 1,1 0,0-1,0 1,1 0,-1 1,0-1,0 0,1 1,-1 0,1 0,0 0,-1 0,1 0,-1 1,7-1,78 3,-58-1,-14 0,0 1,0 0,0 1,0 0,0 1,-1 1,0 0,26 13,-7 1,-1 0,43 37,-67-51,0 0,0 1,0-1,0-1,1 0,0 0,-1 0,2-2,-2 0,2 0,17 2,10-1</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7303,16 +7303,16 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">411 1540</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1956.99">463 957,'0'1,"1"-1,0 0,0 0,-1 0,1 1,0-1,-1 0,1 1,0-1,-1 0,1 1,0-1,-1 1,1-1,-1 1,1 0,-1-1,1 1,-1-1,1 1,-1 0,1-1,-1 1,0 0,0 0,1-1,-1 1,0 0,0 0,0-1,0 1,0 1,-1 28,-7-1,-1-1,-1-1,-2 1,0-2,-26 39,-2 8,37-67,-65 144,61-130,1 1,0 0,2 0,0 0,-1 34,4-39,0 20,1 0,1 0,10 55,-9-80,1-1,0 1,1-1,0 0,0 0,1 0,1-1,0 1,0-1,0-1,1 1,1-1,-1 0,1-1,1 0,9 7,-1-3,2-1,-1-1,1-1,1 0,-1-2,1 0,1-1,-1-1,36 3,12-5,110-8,-171 5,-1 1,0-1,0 0,0-1,0 0,0 0,0 0,0 0,-1-1,1 0,-1 0,0-1,0 1,0-1,7-7,-6 4,-1-1,1 1,-1-1,0 0,-1-1,0 1,0-1,-1 0,3-12,1-15,-2-1,-1 0,-2 0,-3-43,1 58,-5-126,0-72,6 175,2 1,17-81,-20 124,0 1,0-1,0 0,0 1,0-1,0 1,0-1,0 0,0 1,1-1,-1 1,0-1,0 1,0-1,1 1,-1-1,0 1,1-1,-1 1,0-1,1 1,-1-1,0 1,1 0,-1-1,1 1,-1 0,1-1,-1 1,1 0,-1-1,1 1,-1 0,1 0,0 0,-1 0,1 0,-1-1,1 1,0 0,-1 0,1 0,-1 1,1-1,-1 0,1 0,0 0,-1 0,1 0,-1 1,1-1,-1 0,1 1,-1-1,1 0,-1 1,1-1,0 1,2 2,0 1,0-1,0 1,0 0,-1 0,5 8,2 11,-1 1,-1 0,-1 0,5 42,59 698,-61 19,-12-718,-2-1,-4 0,-30 118,6-76,-63 144,93-244,-7 17,-1 0,0-1,-18 24,25-40,0-1,0 0,-1-1,1 1,-1-1,0 0,0 0,0 0,-1 0,1-1,-1 0,0 0,0-1,0 0,0 0,0 0,-11 1,-49 0,-121-11,135 4,16 0,-1-1,1-1,0-3,1 0,-39-17,49 15,0 0,1-2,0-1,1 0,0-2,1-1,-30-30,46 41,1 0,0-1,1 0,-1 0,1 0,1 0,-1-1,2 1,-1-1,1 0,0 0,0 0,1 0,0 0,0-1,1 1,0 0,1 0,0 0,0 0,3-11,4-8,1 0,1 0,1 1,26-44,17-17,4 2,4 3,3 3,3 3,130-112,-144 145,-14 15</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3844.99">2183 1434,'4'5,"7"1,5-1,5 0,3-2,2-1,10-1,13 0,2-1,1-1,-3 1,-1 0,-5 0,1 0,-9 4,-9 2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4301.99">1866 1910,'9'0,"7"0,15 0,11 0,11 0,11 0,3 0,0 0,1 0,-6 0,0 0,-6 0,-8 0,-8 0,-11 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5228">3374 1301,'12'-4,"1"0,0 0,0 1,0 1,1 0,-1 1,1 0,25 3,-34-1,0 0,1 1,-1 0,0 0,0 0,0 0,-1 1,1 0,0 0,-1 0,0 0,0 1,0 0,0 0,-1 0,1 0,-1 0,0 1,0 0,-1-1,1 1,-1 0,0 0,2 9,1 5,-2 0,0 1,0-1,-2 1,-1-1,0 1,-2 0,0-1,-8 35,-5 2,-42 109,30-103,13-34,2 2,-12 42,23-69,0-1,1 1,-1 0,1 0,0 0,-1 0,1-1,0 1,1 0,-1 0,0 0,1-1,0 1,0 0,0 0,0-1,0 1,0-1,0 1,1-1,0 1,-1-1,1 0,0 0,0 0,0 0,0 0,1 0,-1-1,0 1,1-1,-1 1,1-1,-1 0,1 0,0 0,-1 0,1-1,0 1,0-1,4 1,13 1,0-1,0 0,0-2,31-4,-48 5,129-22,-95 16</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5777">4088 1063,'0'5,"0"10,0 21,0 17,0 23,0 16,0 15,-9 21,-17 15,-12 11,-9 1,-2-7,9-11,6-7,9-15,8-29</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7113.02">4750 1566,'3'54,"2"0,3-1,21 76,-4-20,-8-27,-5 0,-2 1,-5 1,-3-1,-4 0,-3 1,-24 120,24-180,-1-2,-1 1,-15 33,12-42,1-14,-1-25,4-16,2 0,2 0,2 0,2 0,9-55,-7 52,83-522,-67 480,5 1,2 1,5 2,61-118,-75 170,1 1,2 1,1 0,0 2,2 0,1 2,1 0,1 2,1 1,31-17,-35 24,-1 2,2 1,-1 0,2 2,-1 1,1 1,0 1,1 1,-1 2,1 0,0 2,0 1,44 6,-57-3,0 1,0 0,0 1,-1 1,0 0,0 1,-1 1,0-1,0 2,0 0,14 15,2 4,-2 1,-1 1,22 35,-34-45,-1 2,-1 0,-1 0,-1 1,-1 0,-1 0,6 35,-7-18,-2 1,-1 0,-4 65,0-97,1-1,-1 1,-1-1,0 1,0-1,0 0,-1 0,-1 0,1 0,-1-1,0 1,-1-1,0 0,-7 8,5-8,-1 0,-1-1,1 1,-1-1,0-1,-1 0,1 0,-1-1,0 0,0-1,-11 2,-40 7,-1-3,0-3,0-2,-69-6,52 1,-268-2,319 3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9660.99">6549 1248,'-1'-31,"2"-1,2 1,0 0,3 0,0 0,21-57,-23 78,0 0,1 1,0-1,0 1,1 1,0-1,1 1,0 0,0 0,1 1,-1 0,2 0,-1 1,1 0,0 1,0 0,1 0,-1 1,1 0,0 1,0 0,0 0,1 1,12-1,-5 2,-1 1,1 1,-1 0,0 2,1 0,-1 0,0 2,22 9,-7-1,-1 2,0 1,34 24,-45-25,-1 1,0 1,-1 0,-1 1,-1 1,17 25,73 131,-94-154,20 36,34 64,156 211,-192-295</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10425.99">7898 719,'-9'9,"-12"8,-21 19,-20 11,-14 13,-16 13,-7 8,1 4,-1 14,-11 22,0 8,14-13,19-22,14-13,12-17,16-13,9-17,8-13</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="54092.25">7951 84,'0'-1,"1"-1,-1 1,1-1,0 1,-1-1,1 1,0-1,0 1,0 0,0-1,0 1,1 0,-1 0,0 0,0 0,1 0,-1 0,1 0,2-1,36-17,-30 15,8-3,1 1,1 0,-1 1,1 1,0 1,24-1,126 6,-75 1,-84-3,-1 1,1 0,-1 0,0 1,0 0,0 1,0 0,0 1,0 0,-1 1,0-1,0 2,0-1,0 1,-1 1,0 0,0 0,-1 0,0 1,0 0,-1 0,0 1,-1 0,1 0,-2 0,1 1,-1-1,-1 1,0 0,0 0,1 13,2 59,-8 109,0-72,0-96,0 1,-1-1,-1 0,-2 0,0 0,-1-1,-1 0,-1 0,-1-1,-1-1,-1 1,-1-2,-1 0,-29 33,36-46,1-1,0 0,-1 0,0-1,0 1,-1-1,1-1,-1 0,0 0,0 0,0-1,0 0,0-1,-11 1,-10 0,0-2,-49-5,76 5,0 0,0 0,-1 0,1 0,0-1,0 1,0-1,0 1,0-1,0 0,0 0,0 0,1 0,-1 0,0 0,0-1,1 1,-1 0,1-1,-1 1,1-1,-2-2,3 2,-1 0,1 0,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,1 0,0 0,-1 0,1 0,0 0,2-2,1-3,0 0,1 0,0 0,1 1,0 0,-1 0,2 1,-1-1,1 1,9-5,-3 4,1 1,-1 0,1 1,0 0,1 1,-1 1,1 0,-1 1,1 1,-1 0,1 1,-1 0,1 1,18 5,-7 1,1 1,-1 1,0 2,-1 0,-1 2,35 24,-40-26,1 0,1-1,-1-1,2 0,-1-2,43 10,36 15,-76-24,1 0,-1-2,1-1,1 0,50 3,-53-9</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">430 1478</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1956.99">484 919,'0'1,"1"-1,0 0,0 0,-1 0,1 1,0-1,-1 0,1 1,0-1,-1 0,1 1,1-1,-2 1,1-1,-1 0,1 1,-1-1,1 1,-1-1,1 1,-1 0,1-1,-1 1,0 0,0 0,1-1,-1 1,0 0,0 0,0-1,0 1,0 1,-1 27,-8-1,0-2,-1 0,-3 1,0-2,-26 38,-3 7,39-65,-68 139,63-124,2 0,0 0,2 0,-1 0,0 33,4-38,0 20,1 0,1-1,11 54,-10-78,1 0,0 0,1 0,0-1,1 1,0 0,1-2,0 2,1-2,-1 0,1 1,2-2,-2 1,1-1,2 0,8 6,0-2,2-2,-1 0,1-1,1-1,-1-1,0 0,2-1,-1-2,38 4,12-5,115-8,-179 5,0 1,-1-1,0 0,1-1,-1 1,0-1,0 0,1 0,-2-1,1 0,-1 0,1-1,-1 1,0 0,8-8,-7 4,-1 0,1 0,0-1,-1 1,-1-2,0 1,0 0,0-1,2-11,1-15,-2 0,0-1,-3 1,-3-42,1 56,-6-121,1-70,6 169,2 1,18-78,-21 119,0 1,0-1,0 0,0 1,0-1,0 1,0-1,0 0,0 1,1-1,-1 1,0-1,0 1,0-1,1 1,-1-1,0 1,1-1,-1 1,0 0,1 0,-1-1,0 1,1 0,-1-1,1 1,-1 0,2-1,-2 1,1 0,-1-1,1 1,-1 0,1 0,0 0,-1 0,1 0,-1-1,1 1,0 0,-1 0,1 0,-1 1,1-1,-1 0,1 0,0 0,-1 0,1 0,-1 1,1-1,-1 0,1 1,-1-1,1 0,-1 1,1-1,0 1,2 1,1 2,-1-1,0 1,0 0,-1 0,5 7,3 11,-2 1,-1 0,0 0,4 41,62 669,-63 19,-13-690,-2 0,-5-1,-31 114,7-73,-67 138,98-235,-7 17,-2 0,1 0,-19 22,25-38,1-2,0 1,-1-1,1 1,-2-1,1-1,0 1,0 0,-2 0,2-1,-1 0,0 0,-1-1,1-1,0 1,0 0,-12 1,-51 0,-127-11,142 5,16-1,-1-1,2-1,-1-3,2 1,-42-17,52 14,0 1,1-3,0 0,1-1,0-1,1-1,-32-29,49 39,1 0,0-1,0 1,0-1,1 0,1 0,-1 0,2 0,-2-1,2 1,0-1,0 0,1 1,0-1,0-1,1 2,0-1,1 0,0 1,0-1,3-10,5-8,0 0,2 0,0 1,28-42,17-17,5 3,4 2,3 3,3 3,136-107,-151 138,-14 16</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3844.99">2283 1377,'4'4,"7"2,6-1,5 0,3-2,2-1,11-1,13 0,2-1,2-1,-4 1,-1 0,-5 0,1 0,-9 3,-10 3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4301.99">1951 1834,'10'0,"6"0,17 0,11 0,11 0,12 0,3 0,0 0,1 0,-6 0,0 0,-7 0,-7 0,-10 0,-10 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5228">3528 1249,'12'-4,"2"0,0 0,-1 2,1 0,0 0,0 1,1 0,25 3,-34-1,-1 0,1 1,-1-1,1 1,-1 0,0 0,-1 1,2 0,-1 0,-1 0,0 0,0 0,0 1,1 0,-2 0,1 0,-1 0,0 0,0 1,-1-1,2 1,-2 0,0 0,2 8,1 5,-2 0,0 2,1-2,-3 1,-1-1,0 2,-2-1,-1-1,-7 34,-6 2,-43 104,31-99,13-32,2 2,-12 40,24-66,0-1,1 1,-1 0,1 0,0 0,-1-1,1 0,0 1,1 0,-1 0,0 0,1-1,0 1,0 0,0-1,0 0,0 1,0-1,0 1,2-1,-1 1,-1-1,1 0,0 0,0 0,0-1,0 1,1 0,-1-1,0 1,2-1,-2 1,1-1,-1 0,1 0,0 0,-1 0,1-1,1 1,-1-1,4 1,14 1,0-1,0 0,0-2,32-4,-50 5,135-21,-99 15</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5777">4274 1020,'0'5,"0"10,0 19,0 17,0 22,0 15,0 15,-9 20,-18 14,-13 11,-9 1,-2-7,9-11,6-6,10-14,8-29</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7113.02">4967 1503,'3'52,"2"0,3-1,23 73,-5-20,-8-25,-6 0,-1 0,-6 2,-3-1,-4-1,-3 2,-26 115,26-173,-1-2,-1 1,-16 32,12-41,2-13,-2-24,5-15,2 0,2-1,2 1,2 0,9-54,-7 51,87-501,-70 460,5 2,3 0,4 2,64-113,-78 164,1 0,2 1,1 0,0 2,2 0,1 2,1 0,2 2,0 1,33-17,-37 24,-1 1,2 2,-1-1,2 2,-1 2,2 0,-1 1,1 2,-1 1,1 0,1 2,-1 1,46 6,-59-4,-1 2,1 0,0 1,-2 1,1-1,-1 2,0 1,-1-1,1 1,0 1,14 14,2 4,-2 1,-1 0,24 35,-37-44,0 2,-2 0,0 0,-2 1,-1 1,0-1,5 33,-6-16,-3 0,-1 0,-4 63,0-93,1-2,-1 2,-1-1,0 0,-1 0,1 0,-1-1,-1 1,1 0,-1-1,0 0,-2 0,1 0,-7 7,4-7,0 0,-2-2,2 2,-1-1,-1-1,0-1,0 1,0-1,0 0,-1-1,-11 1,-42 8,-1-3,1-4,-1-1,-72-6,54 1,-280-2,334 3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9660.99">6848 1198,'-1'-30,"2"0,2 0,0 0,3 0,1 1,21-56,-24 75,0 1,1 0,1 0,-1 0,1 1,0 0,2 0,-1 0,0 1,2 0,-2 0,2 0,0 2,0-1,1 1,-1 0,1 1,0 0,0 0,1 1,-1 0,1 0,0 1,13-1,-5 2,-1 1,1 1,-2 0,1 2,1 0,-1 0,0 2,22 8,-6 0,-2 1,1 2,35 22,-47-24,-2 2,1 0,-1 0,-1 2,-1 0,17 24,77 126,-98-148,20 35,36 61,163 203,-201-284</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10425.99">8258 690,'-9'9,"-13"7,-22 19,-21 10,-14 12,-17 14,-8 6,2 5,-2 13,-11 21,0 8,15-13,19-20,15-14,13-15,16-13,10-17,8-12</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="54092.25">8314 81,'0'-1,"1"-1,-1 1,1-1,0 1,-1-1,1 1,0-1,0 1,0 0,0-1,0 1,1 0,-1 0,0 0,0 0,1 1,-1-1,2 0,1-1,38-17,-32 16,9-4,1 1,1 0,-2 2,2 0,0 1,25-1,132 6,-79 1,-87-3,-2 1,2 0,-2 0,1 1,-1 0,1 0,-1 1,1 1,-1 0,-1 1,1-1,-1 1,1 0,-1 1,-1 1,1-1,-1 1,0 0,-1 0,0 1,-1 0,1 0,-2 1,1 0,-2-1,2 2,-2-1,-1 0,0 1,0-1,1 14,3 55,-9 106,-1-70,1-92,0 1,-1-1,-1 0,-2 0,-1 0,0-1,-1 1,-2-1,0-1,-2-1,0 1,-2-2,0 1,-31 31,37-45,2 0,0 0,-2 0,1-1,0 0,-2 0,2-1,-1 0,-1 0,1 0,0-1,-1 0,1-1,-12 0,-10 1,-1-2,-50-4,79 4,0 0,0 0,-2 0,2 0,0-1,0 1,0-1,0 1,0-1,0 0,0 0,0 0,1 0,-1 0,-1 0,1-1,1 1,-1 0,1-1,-1 1,1-1,-2-2,3 3,-1-1,1 0,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,1 1,0-1,-1 0,1 0,0 0,2-2,1-3,1 1,0-1,0 0,1 1,1 1,-2-1,2 1,-1-1,2 2,8-6,-2 4,1 1,-2 1,2 0,-1 0,2 1,-1 1,1 0,-2 1,2 1,-2 0,2 1,-1 0,0 1,20 5,-8 0,1 2,0 1,-1 1,-1 1,-1 1,37 24,-42-26,0 1,2-2,-1 0,2-1,-1-1,45 9,38 15,-80-23,1-1,-1-1,1-1,1 0,53 2,-56-8</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7366,13 +7366,13 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 717,'9'0,"12"0,16 5,10 1,7-1,3 4,14 5,9 0,-6-3,-9-2,-13-4,-14-2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="798">1060 82,'11'-1,"1"-1,0 0,-1-1,1 0,-1-1,16-7,14-4,-4 4,1 2,1 2,66-5,117 11,-124 2,-70 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2254.01">1033 55,'11'1,"0"0,0 1,0 0,0 1,0 0,0 0,-1 1,16 9,9 6,33 25,-57-36,242 184,-73-52,-150-122,-26-16,1 0,-1 0,1 1,-1-1,0 1,0 1,0-1,0 0,6 8,-10-9,0-1,0 0,0 0,0 0,-1 0,1 0,0 1,-1-1,1 0,-1 0,1 0,-1 0,1 0,-1 0,0 0,1 0,-1-1,0 1,0 0,0 0,0-1,0 1,0 0,0-1,-1 2,-30 17,31-18,-68 39,-102 79,-55 67,8-5,180-153,18-14,0 1,1 1,-17 19,35-34,1-1,-1 1,1-1,-1 1,1-1,-1 1,1-1,-1 1,1-1,-1 1,1 0,0-1,-1 1,1-1,0 1,0 0,0 0,-1-1,1 1,0 0,0-1,0 1,0 0,0-1,0 1,0 0,0 0,1-1,-1 1,0 0,0-1,1 1,-1 0,0-1,1 1,-1-1,0 1,1 0,-1-1,1 1,-1-1,1 1,-1-1,1 0,-1 1,1-1,0 1,-1-1,1 0,0 1,-1-1,1 0,0 0,-1 0,1 0,0 1,-1-1,1 0,0 0,0 0,-1-1,2 1,58 2,-50-2,754-9,-700 5,-42-2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3791.99">2700 505,'0'-10,"0"-1,-1 0,0 1,0-1,-5-16,5 24,0 0,-1 1,1-1,-1 0,1 0,-1 1,0-1,0 1,-1-1,1 1,0 0,-1 0,1 0,-1 0,0 0,1 1,-1-1,0 1,0 0,0 0,0 0,-6-1,-8-2,-1 1,0 1,0 1,-1 0,1 1,0 1,0 1,0 0,0 2,-22 6,30-7,0 1,1-1,-1 2,1 0,0 0,0 0,1 1,-1 1,1-1,1 1,-1 1,1-1,0 1,1 0,0 1,0 0,1 0,0 0,-4 12,6-11,1 1,0 0,1 0,0-1,1 1,0 0,1 0,0 0,0 0,5 15,-1-5,1-1,1-1,0 1,16 27,-12-30,0 0,1-1,0 0,1-1,1 0,0-1,2-1,-1-1,1 0,1 0,0-2,23 11,-25-15,0 0,0-1,1 0,0-1,0-1,0-1,0 0,0-1,0-1,1 0,-1-1,0-1,0 0,0-2,27-8,-22 4,0-2,0 0,-1-1,0-1,-1-1,0-1,-1 0,31-34,-19 14,-2-2,-1-1,33-62,-55 91,0-1,-1 0,0 0,0-1,-1 1,-1-1,1 1,-2-1,1 0,-1-10,-1 14,-1 1,1-1,-1 1,0-1,-1 1,1 0,-1 0,0 0,-1 0,1 0,-1 0,0 0,0 1,-1-1,1 1,-1 0,0 0,0 1,-8-7,-21-11,-1 0,-1 3,-1 0,0 3,-74-21,96 33,0 0,-1 1,0 1,1 0,-1 1,0 1,0 0,1 1,-1 1,1 0,-25 9,-7 6,1 3,-49 30,7-4,39-23,9-7</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4941.99">3309 320,'-2'1,"1"-1,-1 1,1-1,-1 1,1-1,-1 1,1 0,0 0,0 0,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,0 1,0-1,1 0,-1 1,0-1,0 3,-12 34,13-38,-18 62,-26 109,40-130,0-1,5 81,1-48,-2-68,0 1,0 0,1-1,-1 1,1-1,1 0,-1 1,1-1,3 9,-3-11,1 0,-1 0,1 0,-1 0,1-1,0 1,0-1,0 0,0 0,1 0,-1 0,0 0,1-1,6 2,15 6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6498.57">3679 929,'-13'8,"1"-1,0 2,1 0,0 0,0 1,1 0,1 0,-1 1,2 1,-1 0,2 0,0 0,0 1,-9 27,8-18,1 0,1 1,1 0,1 0,1 0,1 0,1 1,3 33,-2-52,1 0,0 0,0-1,0 1,1 0,-1-1,1 0,0 1,0-1,1 0,-1 0,1 0,0 0,0 0,1-1,-1 1,1-1,-1 0,1 0,0 0,0-1,0 1,1-1,-1 0,9 2,0 0,0-1,0-1,0 0,0-1,0 0,0-1,0-1,16-2,-25 3,-1-1,0 0,0-1,0 1,1 0,-1-1,0 0,-1 0,1 0,0 0,0 0,-1 0,0-1,1 1,-1-1,0 0,0 0,0 1,-1-1,3-6,3-7,0 0,7-32,-9 28,1 2,-2 0,0-1,0 0,-2 1,-1-1,0 0,-1-1,-1 1,-1 1,-5-21,6 36,0 0,0 0,-1 0,1 1,-1-1,0 0,0 1,0 0,0-1,0 1,0 0,-1 0,1 0,-1 0,0 0,1 1,-1-1,0 1,0 0,-4-1,-3-1,0 1,-1 0,0 0,-15 1,-8 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7539.55">4182 717,'4'-4,"11"-2,11-5,11 1,4 1,7 2,10 3,0 2,-2 1,-5 0,-7 2,-7-1,-5 0,-3 1,-3-1,0 0,-5-4,-7-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 687,'9'0,"13"0,16 4,11 2,7-1,3 4,15 4,8 0,-5-2,-10-2,-13-5,-14-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="798">1098 79,'11'-1,"2"-1,-1 0,-1-1,2 0,-2-1,17-6,15-5,-5 5,1 1,2 2,67-4,122 10,-128 2,-73 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2254.01">1070 53,'11'1,"1"0,-1 1,0-1,1 2,-1 0,0 0,0 1,16 8,9 7,34 23,-58-35,250 177,-76-50,-155-116,-27-17,2 1,-2 0,1 1,-1-1,0 1,0 1,0-1,1 0,5 7,-10-8,0-1,0 0,0 0,0 0,-1 0,1 0,0 1,-1-1,1 0,-1-1,1 1,-1 0,1 0,-1 0,0 0,1 0,-1-1,0 1,0 0,0 0,0-1,0 1,0 0,-1-1,0 2,-31 16,32-17,-70 37,-106 76,-57 64,8-4,187-147,18-14,0 1,1 2,-17 17,36-32,1-1,-1 1,1-1,-1 1,1-1,-1 1,1-1,-1 1,1-1,-1 1,1 0,0-1,-1 1,1-1,0 1,0 0,0 0,-1-1,1 1,0 0,0-1,0 1,0 0,0-1,0 1,0 0,0-1,1 0,-1 1,0 0,0-1,1 1,-1 0,0-1,1 1,-1-1,0 1,1 0,-1-1,1 1,-1-1,1 1,-1-1,1 0,-1 1,1-1,0 1,-1-1,1 0,0 1,-1-1,1 0,0 0,-1 0,1 0,0 1,-1-1,1 0,0 0,1 0,-2-1,2 1,60 2,-52-2,781-9,-724 5,-45-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3791.99">2796 484,'0'-10,"0"0,-1-1,0 1,0 0,-5-16,5 23,0 0,-1 1,1 0,-2-1,2 0,-1 1,0-1,0 1,-1-1,1 1,0 0,-1 0,1 1,-1-1,0 0,1 1,-2-1,1 1,0 0,0 0,0 0,-6-1,-9-2,-1 1,1 1,-1 2,-1-1,2 1,-1 1,1 0,-1 1,0 2,-22 6,30-7,1 0,1 0,-2 2,2 0,0 0,-1-1,2 2,-1 1,1-1,0 0,0 2,1-1,0 0,0 1,1 1,0-1,1 1,0 0,-5 11,7-11,1 2,0-1,1 1,0-2,1 2,0-1,1 1,0 0,0-1,5 15,-1-5,2-1,0-1,0 2,17 25,-13-29,1 0,0-1,1 1,0-2,2 1,-1-2,3-1,-2 0,2-1,0 1,1-3,23 12,-25-16,-1 1,1-1,1 0,-1-2,1 0,-1-1,1 0,-1-1,1-1,1 0,-2-1,1-1,-1 0,1-2,27-7,-22 3,0-1,0-1,-2 0,1-2,-1 0,-1-2,0 1,32-33,-20 13,-2-1,-1-2,34-58,-57 86,0-1,-1 1,1-1,-1 0,-1 0,-1-1,1 2,-2-2,1 1,-1-11,-1 15,-1 0,1-1,-1 1,0 0,-1 0,1 0,-1 0,0 0,-1 1,1-1,-2 0,1 0,0 1,-1 0,1 0,-1 0,0 0,0 1,-9-6,-21-11,-1 0,-1 2,-2 1,1 3,-77-21,100 32,-1 0,0 2,-1 0,2 0,-2 1,0 1,1 0,0 0,0 2,0 0,-25 9,-8 5,2 3,-52 29,8-4,41-22,8-7</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4941.99">3427 306,'-2'1,"1"-1,-1 1,1-1,-2 1,2-1,-1 1,1 0,0 0,0 0,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,0 1,0-1,1 0,-1 1,0-1,0 2,-13 34,14-37,-18 59,-28 105,42-125,0 0,5 76,1-45,-2-65,0 1,0 0,1-2,-1 2,1-1,1 0,-1 0,1 0,3 9,-3-11,2-1,-2 1,1 0,-1 0,1-1,0 1,0-1,0 0,0 0,1-1,0 1,-1 0,1-1,6 2,16 6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6498.57">3810 890,'-14'7,"2"0,0 2,0-1,1 1,-1 0,2 1,1 0,-2 0,3 2,-1-1,2 1,-1-1,1 2,-10 25,9-17,1 0,1 1,1 0,0 0,2 0,1 0,1 1,3 32,-2-50,1-1,0 1,0-1,0 1,1 0,-1-2,2 1,-1 1,0-1,1 0,-1-1,1 1,0 0,0 0,1-1,-1 1,2-1,-2-1,1 1,0 0,0-1,0 1,1-1,0 0,8 2,1-1,-1 0,0-1,1 0,-1-1,1 0,-1-1,1-1,16-2,-26 3,-1-1,0 0,0-1,0 1,1 0,0 0,-1-1,-1 0,1 0,0 0,0 0,-1 0,0-1,1 1,-1-1,0 1,1-1,-1 1,-1-1,3-6,3-6,0 0,8-31,-10 26,1 3,-2 0,0-1,1 0,-3 0,-1 0,0 0,-1-1,-1 1,-1 0,-6-19,7 34,0 0,0 0,-1 1,1 0,-1-1,0 0,0 1,0 0,0-1,0 1,0 0,-1 0,1 1,-2-1,1 0,1 1,-1-1,0 1,0 0,-4-1,-4-1,1 1,-1 0,-1 0,-15 1,-8 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7539.55">4331 687,'4'-4,"11"-2,12-4,12 0,3 1,8 3,10 2,0 2,-2 1,-5 0,-8 2,-6-1,-6 0,-3 1,-3-1,0 0,-6-4,-6-2</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7739,10 +7739,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7753,13 +7753,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04DCCC4B-0811-4568-9AE1-09D7AE4DDFE9}">
   <dimension ref="A12:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -7782,7 +7782,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>-3</v>
       </c>
@@ -7810,7 +7810,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>-1</v>
       </c>
@@ -7838,7 +7838,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -7866,7 +7866,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>3</v>
       </c>
@@ -7894,7 +7894,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>5</v>
       </c>
@@ -7922,7 +7922,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>7</v>
       </c>
@@ -7950,7 +7950,7 @@
         <v>2156</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <f>SUM(A13:A18)</f>
         <v>12</v>
@@ -7980,7 +7980,7 @@
         <v>2910</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -7997,7 +7997,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>6</v>
       </c>
@@ -8015,7 +8015,7 @@
         <v>1.9999999999999929</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>12</v>
       </c>
@@ -8032,7 +8032,7 @@
         <v>-0.99999999999999645</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>94</v>
       </c>
@@ -8049,7 +8049,7 @@
         <v>0.99999999999999956</v>
       </c>
     </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H35">
         <f>2-2+2*2</f>
         <v>4</v>
@@ -8067,7 +8067,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>